<commit_message>
Added sprint 3 delieverables and sprint retrospective, main point - Team is unhappy with this sprint a lot of work was left undone
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEA8A197-4C9F-4357-8BEF-EBE8E788ECF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D958CA9-C034-4149-AD3B-F5982C67A103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>Project Planner</t>
   </si>
@@ -248,22 +248,91 @@
     <t>Task 13 Define functionality 3</t>
   </si>
   <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
+    <t>T14.1: Revisit the read code, and find code smells.</t>
+  </si>
+  <si>
+    <t>T14.2: Revisit the read code, and find code smells.</t>
+  </si>
+  <si>
+    <t>T14.3: Revisit the read code, and find code smells.</t>
+  </si>
+  <si>
+    <t>T14.4: Revisit the read code, and find code smells.</t>
+  </si>
+  <si>
+    <t>T14.5: Revisit the read code, and find code smells.</t>
+  </si>
+  <si>
+    <t>T14.6: Revisit the read code, and find code smells.</t>
+  </si>
+  <si>
+    <t>T15.1: Document found code smells, and brainstorm possible solutions.</t>
+  </si>
+  <si>
+    <t>T15.2: Document found code smells, and brainstorm possible solutions.</t>
+  </si>
+  <si>
+    <t>T15.3: Document found code smells, and brainstorm possible solutions.</t>
+  </si>
+  <si>
+    <t>T15.4: Document found code smells, and brainstorm possible solutions.</t>
+  </si>
+  <si>
+    <t>T15.5: Document found code smells, and brainstorm possible solutions.</t>
+  </si>
+  <si>
+    <t>T15.6: Document found code smells, and brainstorm possible solutions.</t>
+  </si>
+  <si>
+    <t>T16.1: Revisit the read code, and find design patterns.</t>
+  </si>
+  <si>
+    <t>T16.2: Revisit the read code, and find design patterns.</t>
+  </si>
+  <si>
+    <t>T16.3: Revisit the read code, and find design patterns.</t>
+  </si>
+  <si>
+    <t>T16.5: Revisit the read code, and find design patterns.</t>
+  </si>
+  <si>
+    <t>T16.6: Revisit the read code, and find design patterns.</t>
+  </si>
+  <si>
+    <t>T17.1: Find code blocks, where some design patterns may be implemented.</t>
+  </si>
+  <si>
+    <t>T17.2: Find code blocks, where some design patterns may be implemented.</t>
+  </si>
+  <si>
+    <t>T17.3: Find code blocks, where some design patterns may be implemented.</t>
+  </si>
+  <si>
+    <t>T17.4: Find code blocks, where some design patterns may be implemented.</t>
+  </si>
+  <si>
+    <t>T17.5: Find code blocks, where some design patterns may be implemented.</t>
+  </si>
+  <si>
+    <t>T17.6: Find code blocks, where some design patterns may be implemented.</t>
+  </si>
+  <si>
+    <t>T18.1: Document found design patterns, and think about possible improvements.</t>
+  </si>
+  <si>
+    <t>T18.2: Document found design patterns, and think about possible improvements.</t>
+  </si>
+  <si>
+    <t>T18.3: Document found design patterns, and think about possible improvements.</t>
+  </si>
+  <si>
+    <t>T18.4: Document found design patterns, and think about possible improvements.</t>
+  </si>
+  <si>
+    <t>T18.5: Document found design patterns, and think about possible improvements.</t>
+  </si>
+  <si>
+    <t>T18.6: Document found design patterns, and think about possible improvements.</t>
   </si>
 </sst>
 </file>
@@ -685,7 +754,7 @@
     <cellStyle name="Plan legend" xfId="11" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="12" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -703,16 +772,6 @@
         <bottom style="thin">
           <color theme="7"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1103,10 +1162,10 @@
     <tabColor rgb="FF735773"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BP23"/>
+  <dimension ref="B1:BP72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1"/>
@@ -1141,7 +1200,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="27" t="s">
@@ -1486,10 +1545,10 @@
         <v>4</v>
       </c>
       <c r="G5" s="22">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3">
-        <v>0.66</v>
+        <v>1</v>
       </c>
       <c r="U5" s="23"/>
     </row>
@@ -1631,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:68" ht="30" customHeight="1">
+    <row r="12" spans="2:68" ht="37.5" customHeight="1">
       <c r="B12">
         <v>67775</v>
       </c>
@@ -1694,10 +1753,10 @@
         <v>13</v>
       </c>
       <c r="G14" s="22">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H14" s="3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="2:68" ht="30" customHeight="1">
@@ -1746,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="30" customHeight="1">
+    <row r="17" spans="2:8" ht="28.5" customHeight="1">
       <c r="B17">
         <v>67775</v>
       </c>
@@ -1769,123 +1828,1118 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="30" customHeight="1">
+    <row r="18" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B18">
+        <v>67286</v>
+      </c>
       <c r="C18" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E18" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="22">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G18" s="22">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="30" customHeight="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B19">
+        <v>67763</v>
+      </c>
       <c r="C19" s="21" t="s">
         <v>42</v>
       </c>
       <c r="D19" s="22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E19" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="22">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G19" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B20">
+        <v>67775</v>
+      </c>
       <c r="C20" s="21" t="s">
         <v>43</v>
       </c>
       <c r="D20" s="22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E20" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F20" s="22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G20" s="22">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B21">
+        <v>67804</v>
+      </c>
       <c r="C21" s="21" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E21" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="22">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G21" s="22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="30" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B22">
+        <v>68130</v>
+      </c>
       <c r="C22" s="21" t="s">
         <v>45</v>
       </c>
       <c r="D22" s="22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E22" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="22">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G22" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="30" customHeight="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B23">
+        <v>68547</v>
+      </c>
       <c r="C23" s="21" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E23" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="22">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G23" s="22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B24">
+        <v>67286</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="22">
+        <v>22</v>
+      </c>
+      <c r="E24" s="22">
+        <v>3</v>
+      </c>
+      <c r="F24" s="22">
+        <v>26</v>
+      </c>
+      <c r="G24" s="22">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B25">
+        <v>67763</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="22">
+        <v>22</v>
+      </c>
+      <c r="E25" s="22">
+        <v>3</v>
+      </c>
+      <c r="F25" s="22">
+        <v>25</v>
+      </c>
+      <c r="G25" s="22">
+        <v>2</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B26">
+        <v>67775</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="22">
+        <v>22</v>
+      </c>
+      <c r="E26" s="22">
+        <v>3</v>
+      </c>
+      <c r="F26" s="22">
+        <v>24</v>
+      </c>
+      <c r="G26" s="22">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B27">
+        <v>67804</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="22">
+        <v>22</v>
+      </c>
+      <c r="E27" s="22">
+        <v>3</v>
+      </c>
+      <c r="F27" s="22">
+        <v>23</v>
+      </c>
+      <c r="G27" s="22">
+        <v>4</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B28">
+        <v>68130</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="22">
+        <v>22</v>
+      </c>
+      <c r="E28" s="22">
+        <v>3</v>
+      </c>
+      <c r="F28" s="22">
+        <v>0</v>
+      </c>
+      <c r="G28" s="22">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B29">
+        <v>68547</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="22">
+        <v>22</v>
+      </c>
+      <c r="E29" s="22">
+        <v>3</v>
+      </c>
+      <c r="F29" s="22">
+        <v>23</v>
+      </c>
+      <c r="G29" s="22">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B30">
+        <v>67286</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="22">
+        <v>20</v>
+      </c>
+      <c r="E30" s="22">
+        <v>2</v>
+      </c>
+      <c r="F30" s="22">
+        <v>21</v>
+      </c>
+      <c r="G30" s="22">
+        <v>6</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B31">
+        <v>67763</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="22">
+        <v>20</v>
+      </c>
+      <c r="E31" s="22">
+        <v>2</v>
+      </c>
+      <c r="F31" s="22">
+        <v>24</v>
+      </c>
+      <c r="G31" s="22">
+        <v>3</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B32">
+        <v>67775</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="22">
+        <v>20</v>
+      </c>
+      <c r="E32" s="22">
+        <v>2</v>
+      </c>
+      <c r="F32" s="22">
+        <v>24</v>
+      </c>
+      <c r="G32" s="22">
+        <v>3</v>
+      </c>
+      <c r="H32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B33">
+        <v>67804</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="22">
+        <v>20</v>
+      </c>
+      <c r="E33" s="22">
+        <v>2</v>
+      </c>
+      <c r="F33" s="22">
+        <v>26</v>
+      </c>
+      <c r="G33" s="22">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B34">
+        <v>68130</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="22">
+        <v>20</v>
+      </c>
+      <c r="E34" s="22">
+        <v>2</v>
+      </c>
+      <c r="F34" s="22">
+        <v>0</v>
+      </c>
+      <c r="G34" s="22">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B35">
+        <v>68547</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="22">
+        <v>20</v>
+      </c>
+      <c r="E35" s="22">
+        <v>2</v>
+      </c>
+      <c r="F35" s="22">
+        <v>21</v>
+      </c>
+      <c r="G35" s="22">
+        <v>6</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B36">
+        <v>67286</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="22">
+        <v>20</v>
+      </c>
+      <c r="E36" s="22">
+        <v>2</v>
+      </c>
+      <c r="F36" s="22">
+        <v>21</v>
+      </c>
+      <c r="G36" s="22">
+        <v>5</v>
+      </c>
+      <c r="H36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B37">
+        <v>67763</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="22">
+        <v>20</v>
+      </c>
+      <c r="E37" s="22">
+        <v>2</v>
+      </c>
+      <c r="F37" s="22">
+        <v>24</v>
+      </c>
+      <c r="G37" s="22">
+        <v>3</v>
+      </c>
+      <c r="H37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B38">
+        <v>67775</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="22">
+        <v>20</v>
+      </c>
+      <c r="E38" s="22">
+        <v>2</v>
+      </c>
+      <c r="F38" s="22">
+        <v>24</v>
+      </c>
+      <c r="G38" s="22">
+        <v>3</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B39">
+        <v>67804</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="22">
+        <v>20</v>
+      </c>
+      <c r="E39" s="22">
+        <v>2</v>
+      </c>
+      <c r="F39" s="22">
+        <v>26</v>
+      </c>
+      <c r="G39" s="22">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B40">
+        <v>68130</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="22">
+        <v>20</v>
+      </c>
+      <c r="E40" s="22">
+        <v>2</v>
+      </c>
+      <c r="F40" s="22">
+        <v>0</v>
+      </c>
+      <c r="G40" s="22">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B41">
+        <v>68547</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="22">
+        <v>20</v>
+      </c>
+      <c r="E41" s="22">
+        <v>2</v>
+      </c>
+      <c r="F41" s="22">
+        <v>21</v>
+      </c>
+      <c r="G41" s="22">
+        <v>6</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B42">
+        <v>67286</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="22">
+        <v>23</v>
+      </c>
+      <c r="E42" s="22">
+        <v>3</v>
+      </c>
+      <c r="F42" s="22">
+        <v>25</v>
+      </c>
+      <c r="G42" s="22">
+        <v>2</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B43">
+        <v>67763</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="22">
+        <v>23</v>
+      </c>
+      <c r="E43" s="22">
+        <v>3</v>
+      </c>
+      <c r="F43" s="22">
+        <v>25</v>
+      </c>
+      <c r="G43" s="22">
+        <v>2</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B44">
+        <v>67775</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="22">
+        <v>23</v>
+      </c>
+      <c r="E44" s="22">
+        <v>3</v>
+      </c>
+      <c r="F44" s="22">
+        <v>26</v>
+      </c>
+      <c r="G44" s="22">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B45">
+        <v>67804</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="22">
+        <v>23</v>
+      </c>
+      <c r="E45" s="22">
+        <v>3</v>
+      </c>
+      <c r="F45" s="22">
+        <v>0</v>
+      </c>
+      <c r="G45" s="22">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B46">
+        <v>68130</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="22">
+        <v>23</v>
+      </c>
+      <c r="E46" s="22">
+        <v>3</v>
+      </c>
+      <c r="F46" s="22">
+        <v>0</v>
+      </c>
+      <c r="G46" s="22">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B47">
+        <v>68547</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="22">
+        <v>23</v>
+      </c>
+      <c r="E47" s="22">
+        <v>3</v>
+      </c>
+      <c r="F47" s="22">
+        <v>24</v>
+      </c>
+      <c r="G47" s="22">
+        <v>3</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="30" customHeight="1">
+      <c r="D48" s="22">
+        <v>0</v>
+      </c>
+      <c r="E48" s="22">
+        <v>0</v>
+      </c>
+      <c r="F48" s="22">
+        <v>0</v>
+      </c>
+      <c r="G48" s="22">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:8" ht="30" customHeight="1">
+      <c r="D49" s="22">
+        <v>0</v>
+      </c>
+      <c r="E49" s="22">
+        <v>0</v>
+      </c>
+      <c r="F49" s="22">
+        <v>0</v>
+      </c>
+      <c r="G49" s="22">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:8" ht="30" customHeight="1">
+      <c r="D50" s="22">
+        <v>0</v>
+      </c>
+      <c r="E50" s="22">
+        <v>0</v>
+      </c>
+      <c r="F50" s="22">
+        <v>0</v>
+      </c>
+      <c r="G50" s="22">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8" ht="30" customHeight="1">
+      <c r="D51" s="22">
+        <v>0</v>
+      </c>
+      <c r="E51" s="22">
+        <v>0</v>
+      </c>
+      <c r="F51" s="22">
+        <v>0</v>
+      </c>
+      <c r="G51" s="22">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8" ht="30" customHeight="1">
+      <c r="D52" s="22">
+        <v>0</v>
+      </c>
+      <c r="E52" s="22">
+        <v>0</v>
+      </c>
+      <c r="F52" s="22">
+        <v>0</v>
+      </c>
+      <c r="G52" s="22">
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8" ht="30" customHeight="1">
+      <c r="D53" s="22">
+        <v>0</v>
+      </c>
+      <c r="E53" s="22">
+        <v>0</v>
+      </c>
+      <c r="F53" s="22">
+        <v>0</v>
+      </c>
+      <c r="G53" s="22">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:8" ht="30" customHeight="1">
+      <c r="D54" s="22">
+        <v>0</v>
+      </c>
+      <c r="E54" s="22">
+        <v>0</v>
+      </c>
+      <c r="F54" s="22">
+        <v>0</v>
+      </c>
+      <c r="G54" s="22">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:8" ht="30" customHeight="1">
+      <c r="D55" s="22">
+        <v>0</v>
+      </c>
+      <c r="E55" s="22">
+        <v>0</v>
+      </c>
+      <c r="F55" s="22">
+        <v>0</v>
+      </c>
+      <c r="G55" s="22">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:8" ht="30" customHeight="1">
+      <c r="D56" s="22">
+        <v>0</v>
+      </c>
+      <c r="E56" s="22">
+        <v>0</v>
+      </c>
+      <c r="F56" s="22">
+        <v>0</v>
+      </c>
+      <c r="G56" s="22">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:8" ht="30" customHeight="1">
+      <c r="D57" s="22">
+        <v>0</v>
+      </c>
+      <c r="E57" s="22">
+        <v>0</v>
+      </c>
+      <c r="F57" s="22">
+        <v>0</v>
+      </c>
+      <c r="G57" s="22">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:8" ht="30" customHeight="1">
+      <c r="D58" s="22">
+        <v>0</v>
+      </c>
+      <c r="E58" s="22">
+        <v>0</v>
+      </c>
+      <c r="F58" s="22">
+        <v>0</v>
+      </c>
+      <c r="G58" s="22">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:8" ht="30" customHeight="1">
+      <c r="D59" s="22">
+        <v>0</v>
+      </c>
+      <c r="E59" s="22">
+        <v>0</v>
+      </c>
+      <c r="F59" s="22">
+        <v>0</v>
+      </c>
+      <c r="G59" s="22">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:8" ht="30" customHeight="1">
+      <c r="D60" s="22">
+        <v>0</v>
+      </c>
+      <c r="E60" s="22">
+        <v>0</v>
+      </c>
+      <c r="F60" s="22">
+        <v>0</v>
+      </c>
+      <c r="G60" s="22">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="4:8" ht="30" customHeight="1">
+      <c r="D61" s="22">
+        <v>0</v>
+      </c>
+      <c r="E61" s="22">
+        <v>0</v>
+      </c>
+      <c r="F61" s="22">
+        <v>0</v>
+      </c>
+      <c r="G61" s="22">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="4:8" ht="30" customHeight="1">
+      <c r="D62" s="22">
+        <v>0</v>
+      </c>
+      <c r="E62" s="22">
+        <v>0</v>
+      </c>
+      <c r="F62" s="22">
+        <v>0</v>
+      </c>
+      <c r="G62" s="22">
+        <v>0</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="4:8" ht="30" customHeight="1">
+      <c r="D63" s="22">
+        <v>0</v>
+      </c>
+      <c r="E63" s="22">
+        <v>0</v>
+      </c>
+      <c r="F63" s="22">
+        <v>0</v>
+      </c>
+      <c r="G63" s="22">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="4:8" ht="30" customHeight="1">
+      <c r="D64" s="22">
+        <v>0</v>
+      </c>
+      <c r="E64" s="22">
+        <v>0</v>
+      </c>
+      <c r="F64" s="22">
+        <v>0</v>
+      </c>
+      <c r="G64" s="22">
+        <v>0</v>
+      </c>
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="4:8" ht="30" customHeight="1">
+      <c r="D65" s="22">
+        <v>0</v>
+      </c>
+      <c r="E65" s="22">
+        <v>0</v>
+      </c>
+      <c r="F65" s="22">
+        <v>0</v>
+      </c>
+      <c r="G65" s="22">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="4:8" ht="30" customHeight="1">
+      <c r="D66" s="22">
+        <v>0</v>
+      </c>
+      <c r="E66" s="22">
+        <v>0</v>
+      </c>
+      <c r="F66" s="22">
+        <v>0</v>
+      </c>
+      <c r="G66" s="22">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="4:8" ht="30" customHeight="1">
+      <c r="D67" s="22">
+        <v>0</v>
+      </c>
+      <c r="E67" s="22">
+        <v>0</v>
+      </c>
+      <c r="F67" s="22">
+        <v>0</v>
+      </c>
+      <c r="G67" s="22">
+        <v>0</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="4:8" ht="30" customHeight="1">
+      <c r="D68" s="22">
+        <v>0</v>
+      </c>
+      <c r="E68" s="22">
+        <v>0</v>
+      </c>
+      <c r="F68" s="22">
+        <v>0</v>
+      </c>
+      <c r="G68" s="22">
+        <v>0</v>
+      </c>
+      <c r="H68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="4:8" ht="30" customHeight="1">
+      <c r="D69" s="22">
+        <v>0</v>
+      </c>
+      <c r="E69" s="22">
+        <v>0</v>
+      </c>
+      <c r="F69" s="22">
+        <v>0</v>
+      </c>
+      <c r="G69" s="22">
+        <v>0</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="4:8" ht="30" customHeight="1">
+      <c r="D70" s="22">
+        <v>0</v>
+      </c>
+      <c r="E70" s="22">
+        <v>0</v>
+      </c>
+      <c r="F70" s="22">
+        <v>0</v>
+      </c>
+      <c r="G70" s="22">
+        <v>0</v>
+      </c>
+      <c r="H70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="4:8" ht="30" customHeight="1">
+      <c r="D71" s="22">
+        <v>0</v>
+      </c>
+      <c r="E71" s="22">
+        <v>0</v>
+      </c>
+      <c r="F71" s="22">
+        <v>0</v>
+      </c>
+      <c r="G71" s="22">
+        <v>0</v>
+      </c>
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="4:8" ht="30" customHeight="1">
+      <c r="D72" s="22">
+        <v>0</v>
+      </c>
+      <c r="E72" s="22">
+        <v>0</v>
+      </c>
+      <c r="F72" s="22">
+        <v>0</v>
+      </c>
+      <c r="G72" s="22">
+        <v>0</v>
+      </c>
+      <c r="H72" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1904,35 +2958,30 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I5:BP23">
-    <cfRule type="expression" dxfId="9" priority="2">
+  <conditionalFormatting sqref="I5:BP72">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="1" priority="9">
       <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24:BP24">
-    <cfRule type="expression" dxfId="1" priority="10">
-      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BP4">

</xml_diff>

<commit_message>
Correct 10/11, management version
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\UNI\y3\ES\Proj\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD772330-4F86-4C8A-855A-63CED18524F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E661354-48B2-4858-8DAF-CDC60B7CE16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>Project Planner</t>
   </si>
@@ -404,19 +404,16 @@
     <t>T24: Review and look into what a Use case diagram covering leakage added feature would look like.</t>
   </si>
   <si>
-    <t>T25: Look into what a Use case diagram covering undo/redo added feature would look like.</t>
-  </si>
-  <si>
-    <t>T26: Go over milestone 2 reviews and identify issues that can be worked on.</t>
-  </si>
-  <si>
-    <t>T27: identify areas of code relating to leaks.</t>
-  </si>
-  <si>
-    <t>T28: identify areas of code to help with use case diagrams</t>
-  </si>
-  <si>
-    <t>T29: identify areas of code to help with use sequence diagrams</t>
+    <t>T27: Work on implementing US1 (Undo / Redo).</t>
+  </si>
+  <si>
+    <t>T28: Work on implementing US2 (Leaks).</t>
+  </si>
+  <si>
+    <t>T25: Go over milestone 2 reviews and identify issues that can be worked on.</t>
+  </si>
+  <si>
+    <t>T26: identify areas of code relating to leaks.</t>
   </si>
 </sst>
 </file>
@@ -651,7 +648,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -709,25 +706,11 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="17" applyBorder="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyBorder="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -795,8 +778,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="17" applyBorder="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="20">
     <cellStyle name="% complete" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="% complete (beyond plan) legend" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Activity" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -810,6 +814,7 @@
     <cellStyle name="Excel Built-in Title" xfId="13" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Label" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Percent Complete" xfId="7" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Period Headers" xfId="8" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="9" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
@@ -817,82 +822,7 @@
     <cellStyle name="Plan legend" xfId="11" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="12" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
-  <dxfs count="75">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -939,89 +869,6 @@
         <top/>
         <bottom style="thin">
           <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
         </bottom>
       </border>
     </dxf>
@@ -1107,55 +954,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7"/>
         </patternFill>
       </fill>
@@ -1165,829 +963,6 @@
         <top/>
         <bottom style="thin">
           <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="7"/>
         </bottom>
       </border>
     </dxf>
@@ -2257,414 +1232,414 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A66" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="39.5" customWidth="1"/>
-    <col min="3" max="3" width="49.83203125" style="6" customWidth="1"/>
-    <col min="4" max="7" width="11.5" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="8" customWidth="1"/>
-    <col min="9" max="28" width="3.25" style="7"/>
+    <col min="3" max="3" width="49.83203125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="11.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="3" customWidth="1"/>
+    <col min="9" max="28" width="3.25" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:68" ht="60" customHeight="1" x14ac:dyDescent="1.2">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="2:68" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="13">
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="8">
         <v>34</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="5" t="s">
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="5" t="s">
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="5" t="s">
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="18"/>
-      <c r="AJ2" s="4" t="s">
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4"/>
-      <c r="AP2" s="4"/>
-      <c r="AQ2" s="4"/>
-    </row>
-    <row r="3" spans="2:68" s="19" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3" t="s">
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+      <c r="AQ2" s="27"/>
+    </row>
+    <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20" t="s">
+      <c r="J3" s="16"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Z3" s="22" t="s">
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Z3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="AB3" s="20" t="s">
+      <c r="AB3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="AI3" s="20" t="s">
+      <c r="AI3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AJ3" s="20"/>
-      <c r="AK3" s="20"/>
-      <c r="AL3" s="20"/>
-      <c r="AM3" s="20"/>
-      <c r="AN3" s="22" t="s">
+      <c r="AJ3" s="15"/>
+      <c r="AK3" s="15"/>
+      <c r="AL3" s="15"/>
+      <c r="AM3" s="15"/>
+      <c r="AN3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="AO3" s="20"/>
-      <c r="AP3" s="20" t="s">
+      <c r="AO3" s="15"/>
+      <c r="AP3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AQ3" s="20"/>
-      <c r="AR3" s="20"/>
-      <c r="AS3" s="20"/>
-      <c r="AT3" s="20"/>
-      <c r="AU3" s="20"/>
-      <c r="AV3" s="20"/>
-      <c r="AW3" s="20" t="s">
+      <c r="AQ3" s="15"/>
+      <c r="AR3" s="15"/>
+      <c r="AS3" s="15"/>
+      <c r="AT3" s="15"/>
+      <c r="AU3" s="15"/>
+      <c r="AV3" s="15"/>
+      <c r="AW3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AX3" s="20"/>
-      <c r="AY3" s="20"/>
-      <c r="AZ3" s="20"/>
-      <c r="BA3" s="20"/>
-      <c r="BB3" s="20"/>
-      <c r="BC3" s="20"/>
-      <c r="BD3" s="20" t="s">
+      <c r="AX3" s="15"/>
+      <c r="AY3" s="15"/>
+      <c r="AZ3" s="15"/>
+      <c r="BA3" s="15"/>
+      <c r="BB3" s="15"/>
+      <c r="BC3" s="15"/>
+      <c r="BD3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="BE3" s="20"/>
-      <c r="BF3" s="20"/>
-      <c r="BG3" s="20"/>
-      <c r="BH3" s="20"/>
-      <c r="BI3" s="20"/>
-      <c r="BJ3" s="20"/>
-      <c r="BK3" s="20"/>
-      <c r="BL3" s="20"/>
-      <c r="BM3" s="20"/>
-      <c r="BN3" s="22" t="s">
+      <c r="BE3" s="15"/>
+      <c r="BF3" s="15"/>
+      <c r="BG3" s="15"/>
+      <c r="BH3" s="15"/>
+      <c r="BI3" s="15"/>
+      <c r="BJ3" s="15"/>
+      <c r="BK3" s="15"/>
+      <c r="BL3" s="15"/>
+      <c r="BM3" s="15"/>
+      <c r="BN3" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="23">
-        <v>1</v>
-      </c>
-      <c r="J4" s="23">
-        <v>2</v>
-      </c>
-      <c r="K4" s="23">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="18">
+        <v>1</v>
+      </c>
+      <c r="J4" s="18">
+        <v>2</v>
+      </c>
+      <c r="K4" s="18">
         <v>3</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="18">
         <v>4</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="18">
         <v>5</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="18">
         <v>6</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="18">
         <v>7</v>
       </c>
-      <c r="P4" s="23">
+      <c r="P4" s="18">
         <v>8</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="18">
         <v>9</v>
       </c>
-      <c r="R4" s="23">
+      <c r="R4" s="18">
         <v>10</v>
       </c>
-      <c r="S4" s="23">
+      <c r="S4" s="18">
         <v>11</v>
       </c>
-      <c r="T4" s="23">
+      <c r="T4" s="18">
         <v>12</v>
       </c>
-      <c r="U4" s="23">
+      <c r="U4" s="18">
         <v>13</v>
       </c>
-      <c r="V4" s="23">
+      <c r="V4" s="18">
         <v>14</v>
       </c>
-      <c r="W4" s="23">
+      <c r="W4" s="18">
         <v>15</v>
       </c>
-      <c r="X4" s="23">
+      <c r="X4" s="18">
         <v>16</v>
       </c>
-      <c r="Y4" s="23">
+      <c r="Y4" s="18">
         <v>17</v>
       </c>
-      <c r="Z4" s="23">
+      <c r="Z4" s="18">
         <v>18</v>
       </c>
-      <c r="AA4" s="23">
+      <c r="AA4" s="18">
         <v>19</v>
       </c>
-      <c r="AB4" s="23">
+      <c r="AB4" s="18">
         <v>20</v>
       </c>
-      <c r="AC4" s="23">
+      <c r="AC4" s="18">
         <v>21</v>
       </c>
-      <c r="AD4" s="23">
+      <c r="AD4" s="18">
         <v>22</v>
       </c>
-      <c r="AE4" s="23">
+      <c r="AE4" s="18">
         <v>23</v>
       </c>
-      <c r="AF4" s="23">
+      <c r="AF4" s="18">
         <v>24</v>
       </c>
-      <c r="AG4" s="23">
+      <c r="AG4" s="18">
         <v>25</v>
       </c>
-      <c r="AH4" s="23">
+      <c r="AH4" s="18">
         <v>26</v>
       </c>
-      <c r="AI4" s="23">
+      <c r="AI4" s="18">
         <v>27</v>
       </c>
-      <c r="AJ4" s="23">
+      <c r="AJ4" s="18">
         <v>28</v>
       </c>
-      <c r="AK4" s="23">
+      <c r="AK4" s="18">
         <v>29</v>
       </c>
-      <c r="AL4" s="23">
+      <c r="AL4" s="18">
         <v>30</v>
       </c>
-      <c r="AM4" s="23">
+      <c r="AM4" s="18">
         <v>31</v>
       </c>
-      <c r="AN4" s="23">
+      <c r="AN4" s="18">
         <v>32</v>
       </c>
-      <c r="AO4" s="23">
+      <c r="AO4" s="18">
         <v>33</v>
       </c>
-      <c r="AP4" s="23">
+      <c r="AP4" s="18">
         <v>34</v>
       </c>
-      <c r="AQ4" s="23">
+      <c r="AQ4" s="18">
         <v>35</v>
       </c>
-      <c r="AR4" s="23">
+      <c r="AR4" s="18">
         <v>36</v>
       </c>
-      <c r="AS4" s="23">
+      <c r="AS4" s="18">
         <v>37</v>
       </c>
-      <c r="AT4" s="23">
+      <c r="AT4" s="18">
         <v>38</v>
       </c>
-      <c r="AU4" s="23">
+      <c r="AU4" s="18">
         <v>39</v>
       </c>
-      <c r="AV4" s="23">
+      <c r="AV4" s="18">
         <v>40</v>
       </c>
-      <c r="AW4" s="23">
+      <c r="AW4" s="18">
         <v>41</v>
       </c>
-      <c r="AX4" s="23">
+      <c r="AX4" s="18">
         <v>42</v>
       </c>
-      <c r="AY4" s="23">
+      <c r="AY4" s="18">
         <v>43</v>
       </c>
-      <c r="AZ4" s="23">
+      <c r="AZ4" s="18">
         <v>44</v>
       </c>
-      <c r="BA4" s="23">
+      <c r="BA4" s="18">
         <v>45</v>
       </c>
-      <c r="BB4" s="23">
+      <c r="BB4" s="18">
         <v>46</v>
       </c>
-      <c r="BC4" s="23">
+      <c r="BC4" s="18">
         <v>47</v>
       </c>
-      <c r="BD4" s="23">
+      <c r="BD4" s="18">
         <v>48</v>
       </c>
-      <c r="BE4" s="23">
+      <c r="BE4" s="18">
         <v>49</v>
       </c>
-      <c r="BF4" s="23">
+      <c r="BF4" s="18">
         <v>50</v>
       </c>
-      <c r="BG4" s="23">
+      <c r="BG4" s="18">
         <v>51</v>
       </c>
-      <c r="BH4" s="23">
+      <c r="BH4" s="18">
         <v>52</v>
       </c>
-      <c r="BI4" s="23">
+      <c r="BI4" s="18">
         <v>53</v>
       </c>
-      <c r="BJ4" s="23">
+      <c r="BJ4" s="18">
         <v>54</v>
       </c>
-      <c r="BK4" s="23">
+      <c r="BK4" s="18">
         <v>55</v>
       </c>
-      <c r="BL4" s="23">
+      <c r="BL4" s="18">
         <v>56</v>
       </c>
-      <c r="BM4" s="23">
+      <c r="BM4" s="18">
         <v>57</v>
       </c>
-      <c r="BN4" s="23">
+      <c r="BN4" s="18">
         <v>58</v>
       </c>
-      <c r="BO4" s="23">
+      <c r="BO4" s="18">
         <v>59</v>
       </c>
-      <c r="BP4" s="23">
+      <c r="BP4" s="18">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="21">
         <v>4</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="21">
         <v>3</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="21">
         <v>4</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="21">
         <v>20</v>
       </c>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="U5" s="27"/>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="U5" s="22"/>
     </row>
     <row r="6" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="21">
         <v>5</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="21">
         <v>6</v>
       </c>
-      <c r="F6" s="26">
-        <v>2</v>
-      </c>
-      <c r="G6" s="26">
+      <c r="F6" s="21">
+        <v>2</v>
+      </c>
+      <c r="G6" s="21">
         <v>16</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2672,22 +1647,22 @@
       <c r="B7">
         <v>67775</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="21">
         <v>8</v>
       </c>
-      <c r="E7" s="26">
-        <v>1</v>
-      </c>
-      <c r="F7" s="26">
+      <c r="E7" s="21">
+        <v>1</v>
+      </c>
+      <c r="F7" s="21">
         <v>3</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="21">
         <v>4</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2695,22 +1670,22 @@
       <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="21">
         <v>9</v>
       </c>
-      <c r="E8" s="26">
-        <v>1</v>
-      </c>
-      <c r="F8" s="26">
+      <c r="E8" s="21">
+        <v>1</v>
+      </c>
+      <c r="F8" s="21">
         <v>7</v>
       </c>
-      <c r="G8" s="26">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="G8" s="21">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2718,22 +1693,22 @@
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="21">
         <v>10</v>
       </c>
-      <c r="E9" s="26">
-        <v>1</v>
-      </c>
-      <c r="F9" s="26">
+      <c r="E9" s="21">
+        <v>1</v>
+      </c>
+      <c r="F9" s="21">
         <v>8</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="21">
         <v>4</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2741,22 +1716,22 @@
       <c r="B10">
         <v>67775</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="21">
         <v>11</v>
       </c>
-      <c r="E10" s="26">
-        <v>2</v>
-      </c>
-      <c r="F10" s="26">
+      <c r="E10" s="21">
+        <v>2</v>
+      </c>
+      <c r="F10" s="21">
         <v>7</v>
       </c>
-      <c r="G10" s="26">
-        <v>2</v>
-      </c>
-      <c r="H10" s="8">
+      <c r="G10" s="21">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2764,22 +1739,22 @@
       <c r="B11">
         <v>67763</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="21">
         <v>13</v>
       </c>
-      <c r="E11" s="26">
-        <v>2</v>
-      </c>
-      <c r="F11" s="26">
+      <c r="E11" s="21">
+        <v>2</v>
+      </c>
+      <c r="F11" s="21">
         <v>13</v>
       </c>
-      <c r="G11" s="26">
-        <v>2</v>
-      </c>
-      <c r="H11" s="8">
+      <c r="G11" s="21">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2787,22 +1762,22 @@
       <c r="B12">
         <v>67775</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="21">
         <v>13</v>
       </c>
-      <c r="E12" s="26">
-        <v>2</v>
-      </c>
-      <c r="F12" s="26">
+      <c r="E12" s="21">
+        <v>2</v>
+      </c>
+      <c r="F12" s="21">
         <v>15</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="21">
         <v>3</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2810,22 +1785,22 @@
       <c r="B13">
         <v>67775</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="21">
         <v>15</v>
       </c>
-      <c r="E13" s="26">
-        <v>2</v>
-      </c>
-      <c r="F13" s="26">
+      <c r="E13" s="21">
+        <v>2</v>
+      </c>
+      <c r="F13" s="21">
         <v>17</v>
       </c>
-      <c r="G13" s="26">
-        <v>2</v>
-      </c>
-      <c r="H13" s="8">
+      <c r="G13" s="21">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2833,22 +1808,22 @@
       <c r="B14">
         <v>68547</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="21">
         <v>13</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="21">
         <v>4</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="21">
         <v>13</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="21">
         <v>14</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="3">
         <v>0.75</v>
       </c>
     </row>
@@ -2856,22 +1831,22 @@
       <c r="B15">
         <v>67775</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="21">
         <v>13</v>
       </c>
-      <c r="E15" s="26">
-        <v>2</v>
-      </c>
-      <c r="F15" s="26">
+      <c r="E15" s="21">
+        <v>2</v>
+      </c>
+      <c r="F15" s="21">
         <v>13</v>
       </c>
-      <c r="G15" s="26">
-        <v>2</v>
-      </c>
-      <c r="H15" s="8">
+      <c r="G15" s="21">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2879,22 +1854,22 @@
       <c r="B16">
         <v>67763</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="21">
         <v>13</v>
       </c>
-      <c r="E16" s="26">
-        <v>2</v>
-      </c>
-      <c r="F16" s="26">
+      <c r="E16" s="21">
+        <v>2</v>
+      </c>
+      <c r="F16" s="21">
         <v>13</v>
       </c>
-      <c r="G16" s="26">
-        <v>2</v>
-      </c>
-      <c r="H16" s="8">
+      <c r="G16" s="21">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2902,22 +1877,22 @@
       <c r="B17">
         <v>67775</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="21">
         <v>14</v>
       </c>
-      <c r="E17" s="26">
-        <v>2</v>
-      </c>
-      <c r="F17" s="26">
+      <c r="E17" s="21">
+        <v>2</v>
+      </c>
+      <c r="F17" s="21">
         <v>15</v>
       </c>
-      <c r="G17" s="26">
-        <v>2</v>
-      </c>
-      <c r="H17" s="8">
+      <c r="G17" s="21">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2925,22 +1900,22 @@
       <c r="B18">
         <v>67286</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="21">
         <v>20</v>
       </c>
-      <c r="E18" s="26">
-        <v>2</v>
-      </c>
-      <c r="F18" s="26">
+      <c r="E18" s="21">
+        <v>2</v>
+      </c>
+      <c r="F18" s="21">
         <v>21</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="21">
         <v>7</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2948,22 +1923,22 @@
       <c r="B19">
         <v>67763</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="21">
         <v>20</v>
       </c>
-      <c r="E19" s="26">
-        <v>2</v>
-      </c>
-      <c r="F19" s="26">
+      <c r="E19" s="21">
+        <v>2</v>
+      </c>
+      <c r="F19" s="21">
         <v>24</v>
       </c>
-      <c r="G19" s="26">
-        <v>2</v>
-      </c>
-      <c r="H19" s="8">
+      <c r="G19" s="21">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2971,22 +1946,22 @@
       <c r="B20">
         <v>67775</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="21">
         <v>20</v>
       </c>
-      <c r="E20" s="26">
-        <v>2</v>
-      </c>
-      <c r="F20" s="26">
+      <c r="E20" s="21">
+        <v>2</v>
+      </c>
+      <c r="F20" s="21">
         <v>20</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="21">
         <v>6</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2994,22 +1969,22 @@
       <c r="B21">
         <v>67804</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="21">
         <v>20</v>
       </c>
-      <c r="E21" s="26">
-        <v>2</v>
-      </c>
-      <c r="F21" s="26">
+      <c r="E21" s="21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="21">
         <v>23</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="21">
         <v>4</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3017,22 +1992,22 @@
       <c r="B22">
         <v>68130</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="21">
         <v>20</v>
       </c>
-      <c r="E22" s="26">
-        <v>2</v>
-      </c>
-      <c r="F22" s="26">
+      <c r="E22" s="21">
+        <v>2</v>
+      </c>
+      <c r="F22" s="21">
         <v>25</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="21">
         <v>3</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3040,22 +2015,22 @@
       <c r="B23">
         <v>68547</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="21">
         <v>20</v>
       </c>
-      <c r="E23" s="26">
-        <v>2</v>
-      </c>
-      <c r="F23" s="26">
+      <c r="E23" s="21">
+        <v>2</v>
+      </c>
+      <c r="F23" s="21">
         <v>21</v>
       </c>
-      <c r="G23" s="26">
-        <v>2</v>
-      </c>
-      <c r="H23" s="8">
+      <c r="G23" s="21">
+        <v>2</v>
+      </c>
+      <c r="H23" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3063,22 +2038,22 @@
       <c r="B24">
         <v>67286</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="21">
         <v>22</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="21">
         <v>3</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="21">
         <v>26</v>
       </c>
-      <c r="G24" s="26">
-        <v>1</v>
-      </c>
-      <c r="H24" s="8">
+      <c r="G24" s="21">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3086,22 +2061,22 @@
       <c r="B25">
         <v>67763</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="21">
         <v>22</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="21">
         <v>3</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="21">
         <v>25</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="21">
         <v>3</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3109,22 +2084,22 @@
       <c r="B26">
         <v>67775</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="21">
         <v>22</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="21">
         <v>3</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="21">
         <v>24</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="21">
         <v>3</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3132,22 +2107,22 @@
       <c r="B27">
         <v>67804</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="21">
         <v>22</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E27" s="21">
         <v>3</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="21">
         <v>23</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="21">
         <v>5</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3155,22 +2130,22 @@
       <c r="B28">
         <v>68130</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="21">
         <v>22</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="21">
         <v>3</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="21">
         <v>27</v>
       </c>
-      <c r="G28" s="26">
-        <v>1</v>
-      </c>
-      <c r="H28" s="8">
+      <c r="G28" s="21">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3178,22 +2153,22 @@
       <c r="B29">
         <v>68547</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="21">
         <v>22</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="21">
         <v>3</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="21">
         <v>23</v>
       </c>
-      <c r="G29" s="26">
+      <c r="G29" s="21">
         <v>4</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3201,22 +2176,22 @@
       <c r="B30">
         <v>67286</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="21">
         <v>20</v>
       </c>
-      <c r="E30" s="26">
-        <v>2</v>
-      </c>
-      <c r="F30" s="26">
+      <c r="E30" s="21">
+        <v>2</v>
+      </c>
+      <c r="F30" s="21">
         <v>21</v>
       </c>
-      <c r="G30" s="26">
+      <c r="G30" s="21">
         <v>6</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3224,22 +2199,22 @@
       <c r="B31">
         <v>67763</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="21">
         <v>20</v>
       </c>
-      <c r="E31" s="26">
-        <v>2</v>
-      </c>
-      <c r="F31" s="26">
+      <c r="E31" s="21">
+        <v>2</v>
+      </c>
+      <c r="F31" s="21">
         <v>24</v>
       </c>
-      <c r="G31" s="26">
+      <c r="G31" s="21">
         <v>3</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3247,22 +2222,22 @@
       <c r="B32">
         <v>67775</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="26">
+      <c r="D32" s="21">
         <v>20</v>
       </c>
-      <c r="E32" s="26">
-        <v>2</v>
-      </c>
-      <c r="F32" s="26">
+      <c r="E32" s="21">
+        <v>2</v>
+      </c>
+      <c r="F32" s="21">
         <v>24</v>
       </c>
-      <c r="G32" s="26">
+      <c r="G32" s="21">
         <v>3</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3270,22 +2245,22 @@
       <c r="B33">
         <v>67804</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="21">
         <v>20</v>
       </c>
-      <c r="E33" s="26">
-        <v>2</v>
-      </c>
-      <c r="F33" s="26">
+      <c r="E33" s="21">
+        <v>2</v>
+      </c>
+      <c r="F33" s="21">
         <v>26</v>
       </c>
-      <c r="G33" s="26">
-        <v>2</v>
-      </c>
-      <c r="H33" s="8">
+      <c r="G33" s="21">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3293,22 +2268,22 @@
       <c r="B34">
         <v>68130</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D34" s="21">
         <v>20</v>
       </c>
-      <c r="E34" s="26">
-        <v>2</v>
-      </c>
-      <c r="F34" s="26">
+      <c r="E34" s="21">
+        <v>2</v>
+      </c>
+      <c r="F34" s="21">
         <v>27</v>
       </c>
-      <c r="G34" s="26">
-        <v>1</v>
-      </c>
-      <c r="H34" s="8">
+      <c r="G34" s="21">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3316,22 +2291,22 @@
       <c r="B35">
         <v>68547</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D35" s="21">
         <v>20</v>
       </c>
-      <c r="E35" s="26">
-        <v>2</v>
-      </c>
-      <c r="F35" s="26">
+      <c r="E35" s="21">
+        <v>2</v>
+      </c>
+      <c r="F35" s="21">
         <v>21</v>
       </c>
-      <c r="G35" s="26">
+      <c r="G35" s="21">
         <v>8</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3339,22 +2314,22 @@
       <c r="B36">
         <v>67286</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="26">
+      <c r="D36" s="21">
         <v>20</v>
       </c>
-      <c r="E36" s="26">
-        <v>2</v>
-      </c>
-      <c r="F36" s="26">
+      <c r="E36" s="21">
+        <v>2</v>
+      </c>
+      <c r="F36" s="21">
         <v>21</v>
       </c>
-      <c r="G36" s="26">
+      <c r="G36" s="21">
         <v>5</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3362,22 +2337,22 @@
       <c r="B37">
         <v>67763</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="26">
+      <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="26">
-        <v>2</v>
-      </c>
-      <c r="F37" s="26">
+      <c r="E37" s="21">
+        <v>2</v>
+      </c>
+      <c r="F37" s="21">
         <v>24</v>
       </c>
-      <c r="G37" s="26">
+      <c r="G37" s="21">
         <v>3</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3385,22 +2360,22 @@
       <c r="B38">
         <v>67775</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="21">
         <v>20</v>
       </c>
-      <c r="E38" s="26">
-        <v>2</v>
-      </c>
-      <c r="F38" s="26">
+      <c r="E38" s="21">
+        <v>2</v>
+      </c>
+      <c r="F38" s="21">
         <v>24</v>
       </c>
-      <c r="G38" s="26">
+      <c r="G38" s="21">
         <v>3</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3408,22 +2383,22 @@
       <c r="B39">
         <v>67804</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="26">
+      <c r="D39" s="21">
         <v>20</v>
       </c>
-      <c r="E39" s="26">
-        <v>2</v>
-      </c>
-      <c r="F39" s="26">
+      <c r="E39" s="21">
+        <v>2</v>
+      </c>
+      <c r="F39" s="21">
         <v>26</v>
       </c>
-      <c r="G39" s="26">
-        <v>2</v>
-      </c>
-      <c r="H39" s="8">
+      <c r="G39" s="21">
+        <v>2</v>
+      </c>
+      <c r="H39" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3431,22 +2406,22 @@
       <c r="B40">
         <v>68130</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="26">
+      <c r="D40" s="21">
         <v>20</v>
       </c>
-      <c r="E40" s="26">
-        <v>2</v>
-      </c>
-      <c r="F40" s="26">
+      <c r="E40" s="21">
+        <v>2</v>
+      </c>
+      <c r="F40" s="21">
         <v>27</v>
       </c>
-      <c r="G40" s="26">
+      <c r="G40" s="21">
         <v>4</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3454,22 +2429,22 @@
       <c r="B41">
         <v>68547</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D41" s="21">
         <v>20</v>
       </c>
-      <c r="E41" s="26">
-        <v>2</v>
-      </c>
-      <c r="F41" s="26">
+      <c r="E41" s="21">
+        <v>2</v>
+      </c>
+      <c r="F41" s="21">
         <v>21</v>
       </c>
-      <c r="G41" s="26">
+      <c r="G41" s="21">
         <v>10</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3477,22 +2452,22 @@
       <c r="B42">
         <v>67286</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="26">
+      <c r="D42" s="21">
         <v>23</v>
       </c>
-      <c r="E42" s="26">
+      <c r="E42" s="21">
         <v>3</v>
       </c>
-      <c r="F42" s="26">
+      <c r="F42" s="21">
         <v>25</v>
       </c>
-      <c r="G42" s="26">
+      <c r="G42" s="21">
         <v>6</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3500,22 +2475,22 @@
       <c r="B43">
         <v>67763</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="26">
+      <c r="D43" s="21">
         <v>23</v>
       </c>
-      <c r="E43" s="26">
+      <c r="E43" s="21">
         <v>3</v>
       </c>
-      <c r="F43" s="26">
+      <c r="F43" s="21">
         <v>25</v>
       </c>
-      <c r="G43" s="26">
+      <c r="G43" s="21">
         <v>3</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3523,22 +2498,22 @@
       <c r="B44">
         <v>67775</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="26">
+      <c r="D44" s="21">
         <v>23</v>
       </c>
-      <c r="E44" s="26">
+      <c r="E44" s="21">
         <v>3</v>
       </c>
-      <c r="F44" s="26">
+      <c r="F44" s="21">
         <v>26</v>
       </c>
-      <c r="G44" s="26">
-        <v>2</v>
-      </c>
-      <c r="H44" s="8">
+      <c r="G44" s="21">
+        <v>2</v>
+      </c>
+      <c r="H44" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3546,22 +2521,22 @@
       <c r="B45">
         <v>67804</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="26">
+      <c r="D45" s="21">
         <v>23</v>
       </c>
-      <c r="E45" s="26">
+      <c r="E45" s="21">
         <v>3</v>
       </c>
-      <c r="F45" s="26">
+      <c r="F45" s="21">
         <v>27</v>
       </c>
-      <c r="G45" s="26">
+      <c r="G45" s="21">
         <v>3</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H45" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3569,22 +2544,22 @@
       <c r="B46">
         <v>68130</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="26">
+      <c r="D46" s="21">
         <v>23</v>
       </c>
-      <c r="E46" s="26">
+      <c r="E46" s="21">
         <v>3</v>
       </c>
-      <c r="F46" s="26">
+      <c r="F46" s="21">
         <v>27</v>
       </c>
-      <c r="G46" s="26">
+      <c r="G46" s="21">
         <v>0</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H46" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3592,22 +2567,22 @@
       <c r="B47">
         <v>68547</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="26">
+      <c r="D47" s="21">
         <v>23</v>
       </c>
-      <c r="E47" s="26">
+      <c r="E47" s="21">
         <v>3</v>
       </c>
-      <c r="F47" s="26">
+      <c r="F47" s="21">
         <v>24</v>
       </c>
-      <c r="G47" s="26">
+      <c r="G47" s="21">
         <v>4</v>
       </c>
-      <c r="H47" s="8">
+      <c r="H47" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3615,22 +2590,22 @@
       <c r="B48">
         <v>67286</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D48" s="21">
         <v>30</v>
       </c>
-      <c r="E48" s="26">
-        <v>1</v>
-      </c>
-      <c r="F48" s="26">
+      <c r="E48" s="21">
+        <v>1</v>
+      </c>
+      <c r="F48" s="21">
         <v>32</v>
       </c>
-      <c r="G48" s="26">
-        <v>1</v>
-      </c>
-      <c r="H48" s="8">
+      <c r="G48" s="21">
+        <v>1</v>
+      </c>
+      <c r="H48" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3638,22 +2613,22 @@
       <c r="B49">
         <v>67763</v>
       </c>
-      <c r="C49" s="25" t="s">
+      <c r="C49" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D49" s="26">
+      <c r="D49" s="21">
         <v>30</v>
       </c>
-      <c r="E49" s="26">
-        <v>1</v>
-      </c>
-      <c r="F49" s="26">
+      <c r="E49" s="21">
+        <v>1</v>
+      </c>
+      <c r="F49" s="21">
         <v>31</v>
       </c>
-      <c r="G49" s="26">
-        <v>1</v>
-      </c>
-      <c r="H49" s="8">
+      <c r="G49" s="21">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3661,22 +2636,22 @@
       <c r="B50">
         <v>67775</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C50" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="26">
+      <c r="D50" s="21">
         <v>30</v>
       </c>
-      <c r="E50" s="26">
-        <v>1</v>
-      </c>
-      <c r="F50" s="26">
+      <c r="E50" s="21">
+        <v>1</v>
+      </c>
+      <c r="F50" s="21">
         <v>31</v>
       </c>
-      <c r="G50" s="26">
-        <v>1</v>
-      </c>
-      <c r="H50" s="8">
+      <c r="G50" s="21">
+        <v>1</v>
+      </c>
+      <c r="H50" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3684,22 +2659,22 @@
       <c r="B51">
         <v>67804</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="C51" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="26">
+      <c r="D51" s="21">
         <v>30</v>
       </c>
-      <c r="E51" s="26">
-        <v>1</v>
-      </c>
-      <c r="F51" s="26">
+      <c r="E51" s="21">
+        <v>1</v>
+      </c>
+      <c r="F51" s="21">
         <v>32</v>
       </c>
-      <c r="G51" s="26">
-        <v>1</v>
-      </c>
-      <c r="H51" s="8">
+      <c r="G51" s="21">
+        <v>1</v>
+      </c>
+      <c r="H51" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3707,22 +2682,22 @@
       <c r="B52">
         <v>68130</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C52" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D52" s="26">
+      <c r="D52" s="21">
         <v>30</v>
       </c>
-      <c r="E52" s="26">
-        <v>1</v>
-      </c>
-      <c r="F52" s="26">
+      <c r="E52" s="21">
+        <v>1</v>
+      </c>
+      <c r="F52" s="21">
         <v>32</v>
       </c>
-      <c r="G52" s="26">
-        <v>1</v>
-      </c>
-      <c r="H52" s="8">
+      <c r="G52" s="21">
+        <v>1</v>
+      </c>
+      <c r="H52" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3730,22 +2705,22 @@
       <c r="B53">
         <v>68547</v>
       </c>
-      <c r="C53" s="25" t="s">
+      <c r="C53" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D53" s="26">
+      <c r="D53" s="21">
         <v>30</v>
       </c>
-      <c r="E53" s="26">
-        <v>1</v>
-      </c>
-      <c r="F53" s="26">
+      <c r="E53" s="21">
+        <v>1</v>
+      </c>
+      <c r="F53" s="21">
         <v>32</v>
       </c>
-      <c r="G53" s="26">
-        <v>1</v>
-      </c>
-      <c r="H53" s="8">
+      <c r="G53" s="21">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3753,22 +2728,22 @@
       <c r="B54">
         <v>67286</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C54" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D54" s="26">
+      <c r="D54" s="21">
         <v>31</v>
       </c>
-      <c r="E54" s="26">
-        <v>2</v>
-      </c>
-      <c r="F54" s="26">
+      <c r="E54" s="21">
+        <v>2</v>
+      </c>
+      <c r="F54" s="21">
         <v>32</v>
       </c>
-      <c r="G54" s="26">
-        <v>1</v>
-      </c>
-      <c r="H54" s="8">
+      <c r="G54" s="21">
+        <v>1</v>
+      </c>
+      <c r="H54" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3776,22 +2751,22 @@
       <c r="B55">
         <v>67763</v>
       </c>
-      <c r="C55" s="25" t="s">
+      <c r="C55" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="26">
+      <c r="D55" s="21">
         <v>30</v>
       </c>
-      <c r="E55" s="26">
-        <v>2</v>
-      </c>
-      <c r="F55" s="26">
+      <c r="E55" s="21">
+        <v>2</v>
+      </c>
+      <c r="F55" s="21">
         <v>32</v>
       </c>
-      <c r="G55" s="26">
-        <v>1</v>
-      </c>
-      <c r="H55" s="8">
+      <c r="G55" s="21">
+        <v>1</v>
+      </c>
+      <c r="H55" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3799,22 +2774,22 @@
       <c r="B56">
         <v>67775</v>
       </c>
-      <c r="C56" s="25" t="s">
+      <c r="C56" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="26">
+      <c r="D56" s="21">
         <v>30</v>
       </c>
-      <c r="E56" s="26">
-        <v>2</v>
-      </c>
-      <c r="F56" s="26">
+      <c r="E56" s="21">
+        <v>2</v>
+      </c>
+      <c r="F56" s="21">
         <v>32</v>
       </c>
-      <c r="G56" s="26">
-        <v>1</v>
-      </c>
-      <c r="H56" s="8">
+      <c r="G56" s="21">
+        <v>1</v>
+      </c>
+      <c r="H56" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3822,22 +2797,22 @@
       <c r="B57">
         <v>67804</v>
       </c>
-      <c r="C57" s="25" t="s">
+      <c r="C57" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D57" s="26">
+      <c r="D57" s="21">
         <v>30</v>
       </c>
-      <c r="E57" s="26">
-        <v>2</v>
-      </c>
-      <c r="F57" s="26">
+      <c r="E57" s="21">
+        <v>2</v>
+      </c>
+      <c r="F57" s="21">
         <v>32</v>
       </c>
-      <c r="G57" s="26">
-        <v>1</v>
-      </c>
-      <c r="H57" s="8">
+      <c r="G57" s="21">
+        <v>1</v>
+      </c>
+      <c r="H57" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3845,22 +2820,22 @@
       <c r="B58">
         <v>68130</v>
       </c>
-      <c r="C58" s="25" t="s">
+      <c r="C58" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D58" s="26">
+      <c r="D58" s="21">
         <v>30</v>
       </c>
-      <c r="E58" s="26">
-        <v>2</v>
-      </c>
-      <c r="F58" s="26">
+      <c r="E58" s="21">
+        <v>2</v>
+      </c>
+      <c r="F58" s="21">
         <v>32</v>
       </c>
-      <c r="G58" s="26">
-        <v>1</v>
-      </c>
-      <c r="H58" s="8">
+      <c r="G58" s="21">
+        <v>1</v>
+      </c>
+      <c r="H58" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3868,22 +2843,22 @@
       <c r="B59">
         <v>68547</v>
       </c>
-      <c r="C59" s="25" t="s">
+      <c r="C59" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D59" s="26">
+      <c r="D59" s="21">
         <v>30</v>
       </c>
-      <c r="E59" s="26">
-        <v>2</v>
-      </c>
-      <c r="F59" s="26">
+      <c r="E59" s="21">
+        <v>2</v>
+      </c>
+      <c r="F59" s="21">
         <v>32</v>
       </c>
-      <c r="G59" s="26">
-        <v>1</v>
-      </c>
-      <c r="H59" s="8">
+      <c r="G59" s="21">
+        <v>1</v>
+      </c>
+      <c r="H59" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3891,22 +2866,22 @@
       <c r="B60">
         <v>67286</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D60" s="26">
+      <c r="D60" s="21">
         <v>28</v>
       </c>
-      <c r="E60" s="26">
-        <v>1</v>
-      </c>
-      <c r="F60" s="26">
+      <c r="E60" s="21">
+        <v>1</v>
+      </c>
+      <c r="F60" s="21">
         <v>28</v>
       </c>
-      <c r="G60" s="26">
-        <v>1</v>
-      </c>
-      <c r="H60" s="8">
+      <c r="G60" s="21">
+        <v>1</v>
+      </c>
+      <c r="H60" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3914,22 +2889,22 @@
       <c r="B61">
         <v>67763</v>
       </c>
-      <c r="C61" s="25" t="s">
+      <c r="C61" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D61" s="26">
+      <c r="D61" s="21">
         <v>28</v>
       </c>
-      <c r="E61" s="26">
-        <v>1</v>
-      </c>
-      <c r="F61" s="26">
+      <c r="E61" s="21">
+        <v>1</v>
+      </c>
+      <c r="F61" s="21">
         <v>28</v>
       </c>
-      <c r="G61" s="26">
-        <v>2</v>
-      </c>
-      <c r="H61" s="8">
+      <c r="G61" s="21">
+        <v>2</v>
+      </c>
+      <c r="H61" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3937,22 +2912,22 @@
       <c r="B62">
         <v>67775</v>
       </c>
-      <c r="C62" s="25" t="s">
+      <c r="C62" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D62" s="26">
+      <c r="D62" s="21">
         <v>28</v>
       </c>
-      <c r="E62" s="26">
-        <v>1</v>
-      </c>
-      <c r="F62" s="26">
+      <c r="E62" s="21">
+        <v>1</v>
+      </c>
+      <c r="F62" s="21">
         <v>28</v>
       </c>
-      <c r="G62" s="26">
-        <v>2</v>
-      </c>
-      <c r="H62" s="8">
+      <c r="G62" s="21">
+        <v>2</v>
+      </c>
+      <c r="H62" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3960,22 +2935,22 @@
       <c r="B63">
         <v>67804</v>
       </c>
-      <c r="C63" s="25" t="s">
+      <c r="C63" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="D63" s="26">
+      <c r="D63" s="21">
         <v>28</v>
       </c>
-      <c r="E63" s="26">
-        <v>1</v>
-      </c>
-      <c r="F63" s="26">
+      <c r="E63" s="21">
+        <v>1</v>
+      </c>
+      <c r="F63" s="21">
         <v>29</v>
       </c>
-      <c r="G63" s="26">
-        <v>1</v>
-      </c>
-      <c r="H63" s="8">
+      <c r="G63" s="21">
+        <v>1</v>
+      </c>
+      <c r="H63" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3983,22 +2958,22 @@
       <c r="B64">
         <v>68130</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="C64" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D64" s="26">
+      <c r="D64" s="21">
         <v>28</v>
       </c>
-      <c r="E64" s="26">
-        <v>1</v>
-      </c>
-      <c r="F64" s="26">
+      <c r="E64" s="21">
+        <v>1</v>
+      </c>
+      <c r="F64" s="21">
         <v>30</v>
       </c>
-      <c r="G64" s="26">
-        <v>1</v>
-      </c>
-      <c r="H64" s="8">
+      <c r="G64" s="21">
+        <v>1</v>
+      </c>
+      <c r="H64" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4006,22 +2981,22 @@
       <c r="B65">
         <v>68547</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D65" s="26">
+      <c r="D65" s="21">
         <v>28</v>
       </c>
-      <c r="E65" s="26">
-        <v>1</v>
-      </c>
-      <c r="F65" s="26">
+      <c r="E65" s="21">
+        <v>1</v>
+      </c>
+      <c r="F65" s="21">
         <v>30</v>
       </c>
-      <c r="G65" s="26">
-        <v>1</v>
-      </c>
-      <c r="H65" s="8">
+      <c r="G65" s="21">
+        <v>1</v>
+      </c>
+      <c r="H65" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4029,22 +3004,22 @@
       <c r="B66">
         <v>67286</v>
       </c>
-      <c r="C66" s="25" t="s">
+      <c r="C66" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D66" s="26">
+      <c r="D66" s="21">
         <v>29</v>
       </c>
-      <c r="E66" s="26">
-        <v>2</v>
-      </c>
-      <c r="F66" s="26">
+      <c r="E66" s="21">
+        <v>2</v>
+      </c>
+      <c r="F66" s="21">
         <v>29</v>
       </c>
-      <c r="G66" s="26">
+      <c r="G66" s="21">
         <v>0</v>
       </c>
-      <c r="H66" s="8">
+      <c r="H66" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4052,22 +3027,22 @@
       <c r="B67">
         <v>67763</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C67" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D67" s="26">
+      <c r="D67" s="21">
         <v>29</v>
       </c>
-      <c r="E67" s="26">
-        <v>2</v>
-      </c>
-      <c r="F67" s="26">
+      <c r="E67" s="21">
+        <v>2</v>
+      </c>
+      <c r="F67" s="21">
         <v>28</v>
       </c>
-      <c r="G67" s="26">
+      <c r="G67" s="21">
         <v>0</v>
       </c>
-      <c r="H67" s="8">
+      <c r="H67" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4075,22 +3050,22 @@
       <c r="B68">
         <v>67775</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D68" s="26">
+      <c r="D68" s="21">
         <v>29</v>
       </c>
-      <c r="E68" s="26">
-        <v>2</v>
-      </c>
-      <c r="F68" s="26">
+      <c r="E68" s="21">
+        <v>2</v>
+      </c>
+      <c r="F68" s="21">
         <v>28</v>
       </c>
-      <c r="G68" s="26">
+      <c r="G68" s="21">
         <v>0</v>
       </c>
-      <c r="H68" s="8">
+      <c r="H68" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4098,22 +3073,22 @@
       <c r="B69">
         <v>67804</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D69" s="26">
+      <c r="D69" s="21">
         <v>29</v>
       </c>
-      <c r="E69" s="26">
-        <v>2</v>
-      </c>
-      <c r="F69" s="26">
+      <c r="E69" s="21">
+        <v>2</v>
+      </c>
+      <c r="F69" s="21">
         <v>29</v>
       </c>
-      <c r="G69" s="26">
+      <c r="G69" s="21">
         <v>0</v>
       </c>
-      <c r="H69" s="8">
+      <c r="H69" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4121,22 +3096,22 @@
       <c r="B70">
         <v>68130</v>
       </c>
-      <c r="C70" s="25" t="s">
+      <c r="C70" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D70" s="26">
+      <c r="D70" s="21">
         <v>29</v>
       </c>
-      <c r="E70" s="26">
-        <v>2</v>
-      </c>
-      <c r="F70" s="26">
+      <c r="E70" s="21">
+        <v>2</v>
+      </c>
+      <c r="F70" s="21">
         <v>30</v>
       </c>
-      <c r="G70" s="26">
+      <c r="G70" s="21">
         <v>0</v>
       </c>
-      <c r="H70" s="8">
+      <c r="H70" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4144,22 +3119,22 @@
       <c r="B71">
         <v>68547</v>
       </c>
-      <c r="C71" s="25" t="s">
+      <c r="C71" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D71" s="26">
+      <c r="D71" s="21">
         <v>29</v>
       </c>
-      <c r="E71" s="26">
-        <v>2</v>
-      </c>
-      <c r="F71" s="26">
+      <c r="E71" s="21">
+        <v>2</v>
+      </c>
+      <c r="F71" s="21">
         <v>30</v>
       </c>
-      <c r="G71" s="26">
+      <c r="G71" s="21">
         <v>0</v>
       </c>
-      <c r="H71" s="8">
+      <c r="H71" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4167,22 +3142,22 @@
       <c r="B72" t="s">
         <v>27</v>
       </c>
-      <c r="C72" s="25" t="s">
+      <c r="C72" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D72" s="26">
+      <c r="D72" s="21">
         <v>34</v>
       </c>
-      <c r="E72" s="26">
+      <c r="E72" s="21">
         <v>3</v>
       </c>
-      <c r="F72" s="26">
+      <c r="F72" s="21">
         <v>0</v>
       </c>
-      <c r="G72" s="26">
+      <c r="G72" s="21">
         <v>0</v>
       </c>
-      <c r="H72" s="8">
+      <c r="H72" s="28">
         <v>0</v>
       </c>
     </row>
@@ -4190,45 +3165,45 @@
       <c r="B73" t="s">
         <v>27</v>
       </c>
-      <c r="C73" s="25" t="s">
+      <c r="C73" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D73" s="7">
+      <c r="D73" s="2">
         <v>34</v>
       </c>
-      <c r="E73" s="26">
-        <v>3</v>
-      </c>
-      <c r="F73" s="26">
+      <c r="E73" s="21">
+        <v>2</v>
+      </c>
+      <c r="F73" s="21">
+        <v>32</v>
+      </c>
+      <c r="G73" s="21">
         <v>0</v>
       </c>
-      <c r="G73" s="26">
-        <v>0</v>
-      </c>
-      <c r="H73" s="8">
-        <v>0</v>
+      <c r="H73" s="28">
+        <v>8.3333333333333301E-2</v>
       </c>
     </row>
     <row r="74" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
         <v>27</v>
       </c>
-      <c r="C74" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D74" s="7">
+      <c r="C74" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D74" s="2">
         <v>34</v>
       </c>
-      <c r="E74" s="26">
+      <c r="E74" s="21">
         <v>3</v>
       </c>
-      <c r="F74" s="26">
+      <c r="F74" s="21">
         <v>0</v>
       </c>
-      <c r="G74" s="26">
+      <c r="G74" s="21">
         <v>0</v>
       </c>
-      <c r="H74" s="8">
+      <c r="H74" s="28">
         <v>0</v>
       </c>
     </row>
@@ -4236,45 +3211,45 @@
       <c r="B75" t="s">
         <v>27</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="7">
+      <c r="C75" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" s="2">
         <v>34</v>
       </c>
-      <c r="E75" s="26">
-        <v>3</v>
-      </c>
-      <c r="F75" s="26">
-        <v>0</v>
-      </c>
-      <c r="G75" s="26">
-        <v>0</v>
-      </c>
-      <c r="H75" s="8">
-        <v>0</v>
+      <c r="E75" s="21">
+        <v>1</v>
+      </c>
+      <c r="F75" s="21">
+        <v>34</v>
+      </c>
+      <c r="G75" s="21">
+        <v>1</v>
+      </c>
+      <c r="H75" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
         <v>27</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D76" s="7">
+      <c r="C76" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D76" s="2">
         <v>34</v>
       </c>
-      <c r="E76" s="26">
+      <c r="E76" s="21">
         <v>3</v>
       </c>
-      <c r="F76" s="26">
+      <c r="F76" s="21">
         <v>0</v>
       </c>
-      <c r="G76" s="26">
+      <c r="G76" s="21">
         <v>0</v>
       </c>
-      <c r="H76" s="8">
+      <c r="H76" s="28">
         <v>0</v>
       </c>
     </row>
@@ -4282,55 +3257,37 @@
       <c r="B77" t="s">
         <v>27</v>
       </c>
-      <c r="C77" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D77" s="26">
+      <c r="C77" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D77" s="21">
         <v>34</v>
       </c>
-      <c r="E77" s="26">
+      <c r="E77" s="21">
         <v>3</v>
       </c>
-      <c r="F77" s="26">
-        <v>0</v>
-      </c>
-      <c r="G77" s="26">
-        <v>0</v>
-      </c>
-      <c r="H77" s="8">
-        <v>0</v>
+      <c r="F77" s="21">
+        <v>34</v>
+      </c>
+      <c r="G77" s="21">
+        <v>1</v>
+      </c>
+      <c r="H77" s="29">
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="78" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B78" t="s">
-        <v>27</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D78" s="7">
-        <v>34</v>
-      </c>
-      <c r="E78" s="26">
-        <v>3</v>
-      </c>
-      <c r="F78" s="26">
-        <v>0</v>
-      </c>
-      <c r="G78" s="26">
-        <v>0</v>
-      </c>
-      <c r="H78" s="8">
-        <v>0</v>
-      </c>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
     </row>
     <row r="79" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F79" s="26"/>
-      <c r="G79" s="26"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
     </row>
     <row r="80" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F80" s="26"/>
-      <c r="G80" s="26"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80"/>
@@ -4352,8 +3309,8 @@
       <c r="AB80"/>
     </row>
     <row r="81" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F81" s="26"/>
-      <c r="G81" s="26"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="21"/>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81"/>
@@ -4375,8 +3332,8 @@
       <c r="AB81"/>
     </row>
     <row r="82" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F82" s="26"/>
-      <c r="G82" s="26"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="21"/>
       <c r="J82"/>
       <c r="K82"/>
       <c r="L82"/>
@@ -4398,8 +3355,8 @@
       <c r="AB82"/>
     </row>
     <row r="83" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F83" s="26"/>
-      <c r="G83" s="26"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
       <c r="J83"/>
       <c r="K83"/>
       <c r="L83"/>
@@ -4421,8 +3378,8 @@
       <c r="AB83"/>
     </row>
     <row r="84" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F84" s="26"/>
-      <c r="G84" s="26"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84"/>
@@ -4444,8 +3401,8 @@
       <c r="AB84"/>
     </row>
     <row r="85" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F85" s="26"/>
-      <c r="G85" s="26"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
       <c r="J85"/>
       <c r="K85"/>
       <c r="L85"/>
@@ -4467,8 +3424,8 @@
       <c r="AB85"/>
     </row>
     <row r="86" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F86" s="26"/>
-      <c r="G86" s="26"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="21"/>
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86"/>
@@ -4490,8 +3447,8 @@
       <c r="AB86"/>
     </row>
     <row r="87" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F87" s="26"/>
-      <c r="G87" s="26"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="21"/>
       <c r="J87"/>
       <c r="K87"/>
       <c r="L87"/>
@@ -4513,8 +3470,8 @@
       <c r="AB87"/>
     </row>
     <row r="88" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F88" s="26"/>
-      <c r="G88" s="26"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="21"/>
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88"/>
@@ -4536,8 +3493,8 @@
       <c r="AB88"/>
     </row>
     <row r="89" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F89" s="26"/>
-      <c r="G89" s="26"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="21"/>
       <c r="J89"/>
       <c r="K89"/>
       <c r="L89"/>
@@ -4559,8 +3516,8 @@
       <c r="AB89"/>
     </row>
     <row r="90" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F90" s="26"/>
-      <c r="G90" s="26"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="21"/>
       <c r="J90"/>
       <c r="K90"/>
       <c r="L90"/>
@@ -4582,8 +3539,8 @@
       <c r="AB90"/>
     </row>
     <row r="91" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F91" s="26"/>
-      <c r="G91" s="26"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="21"/>
       <c r="J91"/>
       <c r="K91"/>
       <c r="L91"/>
@@ -4605,8 +3562,8 @@
       <c r="AB91"/>
     </row>
     <row r="92" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F92" s="26"/>
-      <c r="G92" s="26"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="21"/>
       <c r="J92"/>
       <c r="K92"/>
       <c r="L92"/>
@@ -4628,8 +3585,8 @@
       <c r="AB92"/>
     </row>
     <row r="93" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F93" s="26"/>
-      <c r="G93" s="26"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="21"/>
       <c r="J93"/>
       <c r="K93"/>
       <c r="L93"/>
@@ -4651,8 +3608,8 @@
       <c r="AB93"/>
     </row>
     <row r="94" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F94" s="26"/>
-      <c r="G94" s="26"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="21"/>
       <c r="J94"/>
       <c r="K94"/>
       <c r="L94"/>
@@ -4674,8 +3631,8 @@
       <c r="AB94"/>
     </row>
     <row r="95" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F95" s="26"/>
-      <c r="G95" s="26"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="21"/>
       <c r="J95"/>
       <c r="K95"/>
       <c r="L95"/>
@@ -4697,8 +3654,8 @@
       <c r="AB95"/>
     </row>
     <row r="96" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F96" s="26"/>
-      <c r="G96" s="26"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="21"/>
       <c r="J96"/>
       <c r="K96"/>
       <c r="L96"/>
@@ -4720,8 +3677,8 @@
       <c r="AB96"/>
     </row>
     <row r="97" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F97" s="26"/>
-      <c r="G97" s="26"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="21"/>
       <c r="J97"/>
       <c r="K97"/>
       <c r="L97"/>
@@ -4743,8 +3700,8 @@
       <c r="AB97"/>
     </row>
     <row r="98" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F98" s="26"/>
-      <c r="G98" s="26"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="21"/>
       <c r="J98"/>
       <c r="K98"/>
       <c r="L98"/>
@@ -4766,8 +3723,8 @@
       <c r="AB98"/>
     </row>
     <row r="99" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F99" s="26"/>
-      <c r="G99" s="26"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="21"/>
       <c r="J99"/>
       <c r="K99"/>
       <c r="L99"/>
@@ -4789,8 +3746,8 @@
       <c r="AB99"/>
     </row>
     <row r="100" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F100" s="26"/>
-      <c r="G100" s="26"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="21"/>
       <c r="J100"/>
       <c r="K100"/>
       <c r="L100"/>
@@ -4812,8 +3769,8 @@
       <c r="AB100"/>
     </row>
     <row r="101" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F101" s="26"/>
-      <c r="G101" s="26"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="21"/>
       <c r="J101"/>
       <c r="K101"/>
       <c r="L101"/>
@@ -4835,8 +3792,8 @@
       <c r="AB101"/>
     </row>
     <row r="102" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F102" s="26"/>
-      <c r="G102" s="26"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="21"/>
       <c r="J102"/>
       <c r="K102"/>
       <c r="L102"/>
@@ -4858,8 +3815,8 @@
       <c r="AB102"/>
     </row>
     <row r="103" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F103" s="26"/>
-      <c r="G103" s="26"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="21"/>
       <c r="J103"/>
       <c r="K103"/>
       <c r="L103"/>
@@ -4881,8 +3838,8 @@
       <c r="AB103"/>
     </row>
     <row r="104" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F104" s="26"/>
-      <c r="G104" s="26"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="21"/>
       <c r="J104"/>
       <c r="K104"/>
       <c r="L104"/>
@@ -4904,8 +3861,8 @@
       <c r="AB104"/>
     </row>
     <row r="105" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F105" s="26"/>
-      <c r="G105" s="26"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="21"/>
       <c r="J105"/>
       <c r="K105"/>
       <c r="L105"/>
@@ -4927,8 +3884,8 @@
       <c r="AB105"/>
     </row>
     <row r="106" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F106" s="26"/>
-      <c r="G106" s="26"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="21"/>
       <c r="J106"/>
       <c r="K106"/>
       <c r="L106"/>
@@ -4950,8 +3907,8 @@
       <c r="AB106"/>
     </row>
     <row r="107" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F107" s="26"/>
-      <c r="G107" s="26"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="21"/>
       <c r="J107"/>
       <c r="K107"/>
       <c r="L107"/>
@@ -4973,8 +3930,8 @@
       <c r="AB107"/>
     </row>
     <row r="108" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F108" s="26"/>
-      <c r="G108" s="26"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="21"/>
       <c r="J108"/>
       <c r="K108"/>
       <c r="L108"/>
@@ -4996,8 +3953,8 @@
       <c r="AB108"/>
     </row>
     <row r="109" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F109" s="26"/>
-      <c r="G109" s="26"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="21"/>
       <c r="J109"/>
       <c r="K109"/>
       <c r="L109"/>
@@ -5019,8 +3976,8 @@
       <c r="AB109"/>
     </row>
     <row r="110" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F110" s="26"/>
-      <c r="G110" s="26"/>
+      <c r="F110" s="21"/>
+      <c r="G110" s="21"/>
       <c r="J110"/>
       <c r="K110"/>
       <c r="L110"/>
@@ -5042,8 +3999,8 @@
       <c r="AB110"/>
     </row>
     <row r="111" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F111" s="26"/>
-      <c r="G111" s="26"/>
+      <c r="F111" s="21"/>
+      <c r="G111" s="21"/>
       <c r="J111"/>
       <c r="K111"/>
       <c r="L111"/>
@@ -5065,8 +4022,8 @@
       <c r="AB111"/>
     </row>
     <row r="112" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F112" s="26"/>
-      <c r="G112" s="26"/>
+      <c r="F112" s="21"/>
+      <c r="G112" s="21"/>
       <c r="J112"/>
       <c r="K112"/>
       <c r="L112"/>
@@ -5088,8 +4045,8 @@
       <c r="AB112"/>
     </row>
     <row r="113" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F113" s="26"/>
-      <c r="G113" s="26"/>
+      <c r="F113" s="21"/>
+      <c r="G113" s="21"/>
       <c r="J113"/>
       <c r="K113"/>
       <c r="L113"/>
@@ -6079,6 +5036,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -6086,43 +5048,38 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
+  <conditionalFormatting sqref="I5:BD80">
+    <cfRule type="expression" dxfId="8" priority="29">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I4:BP4">
-    <cfRule type="expression" dxfId="17" priority="34">
+    <cfRule type="expression" dxfId="7" priority="34">
       <formula>I$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BP80">
-    <cfRule type="expression" dxfId="16" priority="26">
+    <cfRule type="expression" dxfId="6" priority="26">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="27">
+    <cfRule type="expression" dxfId="5" priority="27">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="28">
+    <cfRule type="expression" dxfId="4" priority="28">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="30">
+    <cfRule type="expression" dxfId="3" priority="30">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="31">
+    <cfRule type="expression" dxfId="2" priority="31">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="32">
+    <cfRule type="expression" dxfId="1" priority="32">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="33">
+    <cfRule type="expression" dxfId="0" priority="33">
       <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BD80">
-    <cfRule type="expression" dxfId="12" priority="29">
-      <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">

</xml_diff>

<commit_message>
small update before 11/11
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\UNI\y3\ES\Proj\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E661354-48B2-4858-8DAF-CDC60B7CE16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5E0FEC-36DD-420E-A108-4374608B0C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -708,7 +708,7 @@
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -778,6 +778,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -786,18 +795,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1232,8 +1229,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="L77" sqref="L77"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B65" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1271,69 +1268,69 @@
         <v>34</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="26" t="s">
+      <c r="W2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="26" t="s">
+      <c r="AB2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="26"/>
-      <c r="AH2" s="26"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="27" t="s">
+      <c r="AJ2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AQ2" s="25"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1408,13 +1405,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3157,7 +3154,7 @@
       <c r="G72" s="21">
         <v>0</v>
       </c>
-      <c r="H72" s="28">
+      <c r="H72" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3180,7 +3177,7 @@
       <c r="G73" s="21">
         <v>0</v>
       </c>
-      <c r="H73" s="28">
+      <c r="H73" s="3">
         <v>8.3333333333333301E-2</v>
       </c>
     </row>
@@ -3203,7 +3200,7 @@
       <c r="G74" s="21">
         <v>0</v>
       </c>
-      <c r="H74" s="28">
+      <c r="H74" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3226,7 +3223,7 @@
       <c r="G75" s="21">
         <v>1</v>
       </c>
-      <c r="H75" s="28">
+      <c r="H75" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3247,10 +3244,10 @@
         <v>0</v>
       </c>
       <c r="G76" s="21">
-        <v>0</v>
-      </c>
-      <c r="H76" s="28">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H76" s="3">
+        <v>0.33333333333333298</v>
       </c>
     </row>
     <row r="77" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -3272,7 +3269,7 @@
       <c r="G77" s="21">
         <v>1</v>
       </c>
-      <c r="H77" s="29">
+      <c r="H77" s="23">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -5036,11 +5033,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5048,6 +5040,11 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="8" priority="29">

</xml_diff>

<commit_message>
small end of 11/11 day update
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\UNI\y3\ES\Proj\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5E0FEC-36DD-420E-A108-4374608B0C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A9E768-86C1-43AE-AB75-82A24ADBA41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1229,8 +1229,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B65" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1265,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="24" t="s">
@@ -3244,10 +3244,10 @@
         <v>0</v>
       </c>
       <c r="G76" s="21">
-        <v>1</v>
-      </c>
-      <c r="H76" s="3">
-        <v>0.33333333333333298</v>
+        <v>2</v>
+      </c>
+      <c r="H76" s="23">
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="77" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
small end of 12/11 day update
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\UNI\y3\ES\Proj\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A9E768-86C1-43AE-AB75-82A24ADBA41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9A4ECF-8042-48CD-A65E-8A70BEF9D3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,12 +781,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -795,6 +789,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1229,7 +1229,7 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1265,72 +1265,72 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="28"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1405,13 +1405,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3171,14 +3171,12 @@
       <c r="E73" s="21">
         <v>2</v>
       </c>
-      <c r="F73" s="21">
-        <v>32</v>
-      </c>
+      <c r="F73" s="21"/>
       <c r="G73" s="21">
         <v>0</v>
       </c>
       <c r="H73" s="3">
-        <v>8.3333333333333301E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -3195,13 +3193,13 @@
         <v>3</v>
       </c>
       <c r="F74" s="21">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G74" s="21">
-        <v>0</v>
-      </c>
-      <c r="H74" s="3">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="H74" s="23">
+        <v>0.25</v>
       </c>
     </row>
     <row r="75" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -3244,10 +3242,10 @@
         <v>0</v>
       </c>
       <c r="G76" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H76" s="23">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -3267,10 +3265,10 @@
         <v>34</v>
       </c>
       <c r="G77" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H77" s="23">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -5033,6 +5031,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5040,11 +5043,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="8" priority="29">

</xml_diff>

<commit_message>
14/11  small management update
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\UNI\y3\ES\Proj\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8229212-B231-4463-8900-77B6837DA3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD96D80-79B8-43A0-A3BD-E4C11396B153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -790,12 +790,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,6 +798,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1238,8 +1238,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B64" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="AS1" sqref="AS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1274,72 +1274,72 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="28"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1414,13 +1414,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3207,10 +3207,10 @@
         <v>32</v>
       </c>
       <c r="G74" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H74" s="23">
-        <v>0.65</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="75" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -3279,7 +3279,7 @@
         <v>2</v>
       </c>
       <c r="H77" s="23">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="78" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -5075,6 +5075,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5082,11 +5087,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="8" priority="29">

</xml_diff>

<commit_message>
15/11  small management update
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\UNI\y3\ES\Proj\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD96D80-79B8-43A0-A3BD-E4C11396B153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAE7756-3583-4D45-A4FC-C1C3CC0699AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -790,6 +790,12 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -798,12 +804,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1238,8 +1238,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="AS1" sqref="AS1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B64" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1274,72 +1274,72 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="27" t="s">
+      <c r="R2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="28" t="s">
+      <c r="AJ2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="28"/>
-      <c r="AQ2" s="28"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AQ2" s="25"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1414,13 +1414,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3296,11 +3296,11 @@
         <v>1</v>
       </c>
       <c r="F78" s="21">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G78" s="21"/>
       <c r="H78" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="79" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -3317,11 +3317,13 @@
         <v>1</v>
       </c>
       <c r="F79" s="21">
-        <v>0</v>
-      </c>
-      <c r="G79" s="21"/>
+        <v>29</v>
+      </c>
+      <c r="G79" s="21">
+        <v>1</v>
+      </c>
       <c r="H79" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -5075,11 +5077,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5087,6 +5084,11 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="8" priority="29">

</xml_diff>

<commit_message>
16/11 update and also some small fixes
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\UNI\y3\ES\Proj\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAE7756-3583-4D45-A4FC-C1C3CC0699AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EB4198-C25C-4918-998F-67C3D4CFFC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
   <si>
     <t>Project Planner</t>
   </si>
@@ -416,13 +416,16 @@
     <t>T24: Look into what a Use case diagram covering leakage added feature would look like.</t>
   </si>
   <si>
-    <t>67286, 67804, 68130, 68547</t>
-  </si>
-  <si>
     <t>T30: Look into relevant code for implementing US4 (copy and its history)</t>
   </si>
   <si>
     <t>T29: Look into relevant code for implementing US3 (turret targeting)</t>
+  </si>
+  <si>
+    <t>67286, 68130</t>
+  </si>
+  <si>
+    <t>67804, 68547</t>
   </si>
 </sst>
 </file>
@@ -790,12 +793,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,6 +801,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1238,8 +1241,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B64" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1274,72 +1277,72 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="28"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1414,13 +1417,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3145,8 +3148,8 @@
       </c>
     </row>
     <row r="72" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B72" t="s">
-        <v>27</v>
+      <c r="B72">
+        <v>67775</v>
       </c>
       <c r="C72" s="20" t="s">
         <v>98</v>
@@ -3164,12 +3167,12 @@
         <v>1</v>
       </c>
       <c r="H72" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B73" t="s">
-        <v>27</v>
+      <c r="B73">
+        <v>67763</v>
       </c>
       <c r="C73" s="20" t="s">
         <v>99</v>
@@ -3187,7 +3190,7 @@
         <v>1</v>
       </c>
       <c r="H73" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
@@ -3210,12 +3213,12 @@
         <v>4</v>
       </c>
       <c r="H74" s="23">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B75" t="s">
-        <v>27</v>
+      <c r="B75">
+        <v>67763</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>97</v>
@@ -3237,8 +3240,8 @@
       </c>
     </row>
     <row r="76" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B76" t="s">
-        <v>27</v>
+      <c r="B76">
+        <v>67775</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>94</v>
@@ -3260,8 +3263,8 @@
       </c>
     </row>
     <row r="77" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B77" t="s">
-        <v>27</v>
+      <c r="B77">
+        <v>67763</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>95</v>
@@ -3279,15 +3282,15 @@
         <v>2</v>
       </c>
       <c r="H77" s="23">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D78" s="2">
         <v>38</v>
@@ -3296,19 +3299,21 @@
         <v>1</v>
       </c>
       <c r="F78" s="21">
-        <v>29</v>
-      </c>
-      <c r="G78" s="21"/>
+        <v>39</v>
+      </c>
+      <c r="G78" s="21">
+        <v>2</v>
+      </c>
       <c r="H78" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
+        <v>102</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D79" s="2">
         <v>38</v>
@@ -3317,10 +3322,10 @@
         <v>1</v>
       </c>
       <c r="F79" s="21">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G79" s="21">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H79" s="3">
         <v>1</v>
@@ -5077,6 +5082,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5084,11 +5094,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="8" priority="29">

</xml_diff>

<commit_message>
first sprint 6's day management update
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\UNI\y3\ES\Proj\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\fct-unl\INFORMATICA\5th_sem\courses\ES\project\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EB4198-C25C-4918-998F-67C3D4CFFC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021BE87A-9DA9-41A1-B358-8A1EBFF21BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
     <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$F1,'Project Planner'!$F1+'Project Planner'!$G1-1)</definedName>
     <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$D1,'Project Planner'!$D1+'Project Planner'!$E1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$D1&gt;0)</definedName>
+    <definedName name="TitleRegion..BO60">'Project Planner'!$C$3:$C$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
-    <definedName name="TitleRegion..BO60">'Project Planner'!$C$3:$C$4</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="116">
   <si>
     <t>Project Planner</t>
   </si>
@@ -426,6 +426,42 @@
   </si>
   <si>
     <t>67804, 68547</t>
+  </si>
+  <si>
+    <t>T31: Work on implementing US3 (turret's targeting).</t>
+  </si>
+  <si>
+    <t>T32: Work on implementing US4 (copy and its history).</t>
+  </si>
+  <si>
+    <t>T33: Look into what a Use Case covering US3 would look like (turret's targeting).</t>
+  </si>
+  <si>
+    <t>T34: Look into what a Use Case covering US4 would look like (copy and its history).</t>
+  </si>
+  <si>
+    <t>T35: Work on the extensive version of US1's use case (undo/redo).</t>
+  </si>
+  <si>
+    <t>T36: Work on the extensive version of US2's use case (liquid leak checking).</t>
+  </si>
+  <si>
+    <t>T37: Work on the extensive version of US3's use case (turret's targeting).</t>
+  </si>
+  <si>
+    <t>T38: Work on the extensive version of US4's use case (copy and its history).</t>
+  </si>
+  <si>
+    <t>T39: Work on the sequence diagram for US1 (undo/redo).</t>
+  </si>
+  <si>
+    <t>T40: Work on the sequence diagram for US2 (liquid leak checking).</t>
+  </si>
+  <si>
+    <t>T41: Look into what a Class Diagram covering US1 would look like (undo/redo).</t>
+  </si>
+  <si>
+    <t>T42: Look into what a class diagram covering US2 would look like (liquid leak checking).</t>
   </si>
 </sst>
 </file>
@@ -793,6 +829,12 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -801,12 +843,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -823,15 +859,635 @@
     <cellStyle name="Excel Built-in Title" xfId="13" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Label" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Percent Complete" xfId="7" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Percentagem" xfId="19" builtinId="5"/>
     <cellStyle name="Period Headers" xfId="8" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Period Highlight Control" xfId="9" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Period Value" xfId="10" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Plan legend" xfId="11" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="12" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="9" tint="0.59978026673177287"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="9" tint="0.59978026673177287"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="9" tint="0.59978026673177287"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="9" tint="0.59978026673177287"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="9" tint="0.59978026673177287"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1241,21 +1897,21 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="L70" sqref="L70"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B88" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="39.5" customWidth="1"/>
-    <col min="3" max="3" width="49.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.875" style="1" customWidth="1"/>
     <col min="4" max="7" width="11.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.5" style="3" customWidth="1"/>
     <col min="9" max="28" width="3.25" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:68" ht="60" customHeight="1" x14ac:dyDescent="1.2">
+    <row r="1" spans="2:68" ht="60" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1921,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="2:68" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:68" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1277,72 +1933,72 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="27" t="s">
+      <c r="R2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="28" t="s">
+      <c r="AJ2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="28"/>
-      <c r="AQ2" s="28"/>
-    </row>
-    <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="26" t="s">
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AQ2" s="25"/>
+    </row>
+    <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1416,14 +2072,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+    <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -1605,7 +2261,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
         <v>25</v>
       </c>
@@ -1629,7 +2285,7 @@
       </c>
       <c r="U5" s="22"/>
     </row>
-    <row r="6" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -1652,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>67775</v>
       </c>
@@ -1675,7 +2331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>30</v>
       </c>
@@ -1698,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>30</v>
       </c>
@@ -1721,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>67775</v>
       </c>
@@ -1744,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>67763</v>
       </c>
@@ -1767,7 +2423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:68" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:68" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>67775</v>
       </c>
@@ -1790,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>67775</v>
       </c>
@@ -1813,7 +2469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:68" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:68" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>68547</v>
       </c>
@@ -1836,7 +2492,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>67775</v>
       </c>
@@ -1859,7 +2515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>67763</v>
       </c>
@@ -1882,7 +2538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>67775</v>
       </c>
@@ -1905,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>67286</v>
       </c>
@@ -1928,7 +2584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>67763</v>
       </c>
@@ -1951,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>67775</v>
       </c>
@@ -1974,7 +2630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>67804</v>
       </c>
@@ -1997,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>68130</v>
       </c>
@@ -2020,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>68547</v>
       </c>
@@ -2043,7 +2699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>67286</v>
       </c>
@@ -2066,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>67763</v>
       </c>
@@ -2089,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>67775</v>
       </c>
@@ -2112,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>67804</v>
       </c>
@@ -2135,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>68130</v>
       </c>
@@ -2158,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>68547</v>
       </c>
@@ -2181,7 +2837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>67286</v>
       </c>
@@ -2204,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>67763</v>
       </c>
@@ -2227,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>67775</v>
       </c>
@@ -2250,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>67804</v>
       </c>
@@ -2273,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>68130</v>
       </c>
@@ -2296,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>68547</v>
       </c>
@@ -2319,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>67286</v>
       </c>
@@ -2342,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>67763</v>
       </c>
@@ -2365,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>67775</v>
       </c>
@@ -2388,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39">
         <v>67804</v>
       </c>
@@ -2411,7 +3067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40">
         <v>68130</v>
       </c>
@@ -2434,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41">
         <v>68547</v>
       </c>
@@ -2457,7 +3113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42">
         <v>67286</v>
       </c>
@@ -2480,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43">
         <v>67763</v>
       </c>
@@ -2503,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44">
         <v>67775</v>
       </c>
@@ -2526,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45">
         <v>67804</v>
       </c>
@@ -2549,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>68130</v>
       </c>
@@ -2572,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47">
         <v>68547</v>
       </c>
@@ -2595,7 +3251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48">
         <v>67286</v>
       </c>
@@ -2618,7 +3274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>67763</v>
       </c>
@@ -2641,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>67775</v>
       </c>
@@ -2664,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>67804</v>
       </c>
@@ -2687,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>68130</v>
       </c>
@@ -2710,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>68547</v>
       </c>
@@ -2733,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>67286</v>
       </c>
@@ -2756,7 +3412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>67763</v>
       </c>
@@ -2779,7 +3435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>67775</v>
       </c>
@@ -2802,7 +3458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>67804</v>
       </c>
@@ -2825,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>68130</v>
       </c>
@@ -2848,7 +3504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59">
         <v>68547</v>
       </c>
@@ -2871,7 +3527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60">
         <v>67286</v>
       </c>
@@ -2894,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>67763</v>
       </c>
@@ -2917,7 +3573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>67775</v>
       </c>
@@ -2940,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>67804</v>
       </c>
@@ -2963,7 +3619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>68130</v>
       </c>
@@ -2986,7 +3642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65">
         <v>68547</v>
       </c>
@@ -3009,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66">
         <v>67286</v>
       </c>
@@ -3032,7 +3688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67">
         <v>67763</v>
       </c>
@@ -3055,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>67775</v>
       </c>
@@ -3078,7 +3734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69">
         <v>67804</v>
       </c>
@@ -3101,7 +3757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70">
         <v>68130</v>
       </c>
@@ -3124,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71">
         <v>68547</v>
       </c>
@@ -3147,7 +3803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>67775</v>
       </c>
@@ -3170,7 +3826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73">
         <v>67763</v>
       </c>
@@ -3193,7 +3849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>27</v>
       </c>
@@ -3216,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75">
         <v>67763</v>
       </c>
@@ -3239,7 +3895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76">
         <v>67775</v>
       </c>
@@ -3262,7 +3918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77">
         <v>67763</v>
       </c>
@@ -3285,7 +3941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>103</v>
       </c>
@@ -3308,7 +3964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>102</v>
       </c>
@@ -3331,7 +3987,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D80" s="2">
+        <v>40</v>
+      </c>
+      <c r="E80" s="2">
+        <v>3</v>
+      </c>
       <c r="F80" s="21"/>
       <c r="G80" s="21"/>
       <c r="J80"/>
@@ -3354,8 +4022,22 @@
       <c r="AA80"/>
       <c r="AB80"/>
     </row>
-    <row r="81" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F81" s="21"/>
+    <row r="81" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>103</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D81" s="2">
+        <v>40</v>
+      </c>
+      <c r="E81" s="2">
+        <v>3</v>
+      </c>
+      <c r="F81" s="21">
+        <v>40</v>
+      </c>
       <c r="G81" s="21"/>
       <c r="J81"/>
       <c r="K81"/>
@@ -3377,8 +4059,22 @@
       <c r="AA81"/>
       <c r="AB81"/>
     </row>
-    <row r="82" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F82" s="21"/>
+    <row r="82" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>102</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D82" s="2">
+        <v>43</v>
+      </c>
+      <c r="E82" s="2">
+        <v>1</v>
+      </c>
+      <c r="F82" s="21">
+        <v>40</v>
+      </c>
       <c r="G82" s="21"/>
       <c r="J82"/>
       <c r="K82"/>
@@ -3400,7 +4096,19 @@
       <c r="AA82"/>
       <c r="AB82"/>
     </row>
-    <row r="83" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" s="2">
+        <v>43</v>
+      </c>
+      <c r="E83" s="2">
+        <v>1</v>
+      </c>
       <c r="F83" s="21"/>
       <c r="G83" s="21"/>
       <c r="J83"/>
@@ -3423,8 +4131,22 @@
       <c r="AA83"/>
       <c r="AB83"/>
     </row>
-    <row r="84" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F84" s="21"/>
+    <row r="84" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>67775</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D84" s="2">
+        <v>40</v>
+      </c>
+      <c r="E84" s="2">
+        <v>3</v>
+      </c>
+      <c r="F84" s="21">
+        <v>40</v>
+      </c>
       <c r="G84" s="21"/>
       <c r="J84"/>
       <c r="K84"/>
@@ -3446,7 +4168,19 @@
       <c r="AA84"/>
       <c r="AB84"/>
     </row>
-    <row r="85" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>67763</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D85" s="2">
+        <v>40</v>
+      </c>
+      <c r="E85" s="2">
+        <v>3</v>
+      </c>
       <c r="F85" s="21"/>
       <c r="G85" s="21"/>
       <c r="J85"/>
@@ -3469,7 +4203,19 @@
       <c r="AA85"/>
       <c r="AB85"/>
     </row>
-    <row r="86" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D86" s="2">
+        <v>44</v>
+      </c>
+      <c r="E86" s="2">
+        <v>3</v>
+      </c>
       <c r="F86" s="21"/>
       <c r="G86" s="21"/>
       <c r="J86"/>
@@ -3492,7 +4238,19 @@
       <c r="AA86"/>
       <c r="AB86"/>
     </row>
-    <row r="87" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>103</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D87" s="2">
+        <v>44</v>
+      </c>
+      <c r="E87" s="2">
+        <v>3</v>
+      </c>
       <c r="F87" s="21"/>
       <c r="G87" s="21"/>
       <c r="J87"/>
@@ -3515,7 +4273,19 @@
       <c r="AA87"/>
       <c r="AB87"/>
     </row>
-    <row r="88" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>67775</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D88" s="2">
+        <v>43</v>
+      </c>
+      <c r="E88" s="2">
+        <v>4</v>
+      </c>
       <c r="F88" s="21"/>
       <c r="G88" s="21"/>
       <c r="J88"/>
@@ -3538,7 +4308,19 @@
       <c r="AA88"/>
       <c r="AB88"/>
     </row>
-    <row r="89" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>67763</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D89" s="2">
+        <v>43</v>
+      </c>
+      <c r="E89" s="2">
+        <v>4</v>
+      </c>
       <c r="F89" s="21"/>
       <c r="G89" s="21"/>
       <c r="J89"/>
@@ -3561,7 +4343,19 @@
       <c r="AA89"/>
       <c r="AB89"/>
     </row>
-    <row r="90" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>67775</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D90" s="2">
+        <v>46</v>
+      </c>
+      <c r="E90" s="2">
+        <v>2</v>
+      </c>
       <c r="F90" s="21"/>
       <c r="G90" s="21"/>
       <c r="J90"/>
@@ -3584,7 +4378,19 @@
       <c r="AA90"/>
       <c r="AB90"/>
     </row>
-    <row r="91" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>67763</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D91" s="2">
+        <v>46</v>
+      </c>
+      <c r="E91" s="2">
+        <v>2</v>
+      </c>
       <c r="F91" s="21"/>
       <c r="G91" s="21"/>
       <c r="J91"/>
@@ -3607,7 +4413,7 @@
       <c r="AA91"/>
       <c r="AB91"/>
     </row>
-    <row r="92" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F92" s="21"/>
       <c r="G92" s="21"/>
       <c r="J92"/>
@@ -3630,7 +4436,7 @@
       <c r="AA92"/>
       <c r="AB92"/>
     </row>
-    <row r="93" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F93" s="21"/>
       <c r="G93" s="21"/>
       <c r="J93"/>
@@ -3653,7 +4459,7 @@
       <c r="AA93"/>
       <c r="AB93"/>
     </row>
-    <row r="94" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F94" s="21"/>
       <c r="G94" s="21"/>
       <c r="J94"/>
@@ -3676,7 +4482,7 @@
       <c r="AA94"/>
       <c r="AB94"/>
     </row>
-    <row r="95" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F95" s="21"/>
       <c r="G95" s="21"/>
       <c r="J95"/>
@@ -3699,7 +4505,7 @@
       <c r="AA95"/>
       <c r="AB95"/>
     </row>
-    <row r="96" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F96" s="21"/>
       <c r="G96" s="21"/>
       <c r="J96"/>
@@ -3722,7 +4528,7 @@
       <c r="AA96"/>
       <c r="AB96"/>
     </row>
-    <row r="97" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F97" s="21"/>
       <c r="G97" s="21"/>
       <c r="J97"/>
@@ -3745,7 +4551,7 @@
       <c r="AA97"/>
       <c r="AB97"/>
     </row>
-    <row r="98" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F98" s="21"/>
       <c r="G98" s="21"/>
       <c r="J98"/>
@@ -3768,7 +4574,7 @@
       <c r="AA98"/>
       <c r="AB98"/>
     </row>
-    <row r="99" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F99" s="21"/>
       <c r="G99" s="21"/>
       <c r="J99"/>
@@ -3791,7 +4597,7 @@
       <c r="AA99"/>
       <c r="AB99"/>
     </row>
-    <row r="100" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F100" s="21"/>
       <c r="G100" s="21"/>
       <c r="J100"/>
@@ -3814,7 +4620,7 @@
       <c r="AA100"/>
       <c r="AB100"/>
     </row>
-    <row r="101" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F101" s="21"/>
       <c r="G101" s="21"/>
       <c r="J101"/>
@@ -3837,7 +4643,7 @@
       <c r="AA101"/>
       <c r="AB101"/>
     </row>
-    <row r="102" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F102" s="21"/>
       <c r="G102" s="21"/>
       <c r="J102"/>
@@ -3860,7 +4666,7 @@
       <c r="AA102"/>
       <c r="AB102"/>
     </row>
-    <row r="103" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F103" s="21"/>
       <c r="G103" s="21"/>
       <c r="J103"/>
@@ -3883,7 +4689,7 @@
       <c r="AA103"/>
       <c r="AB103"/>
     </row>
-    <row r="104" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F104" s="21"/>
       <c r="G104" s="21"/>
       <c r="J104"/>
@@ -3906,7 +4712,7 @@
       <c r="AA104"/>
       <c r="AB104"/>
     </row>
-    <row r="105" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F105" s="21"/>
       <c r="G105" s="21"/>
       <c r="J105"/>
@@ -3929,7 +4735,7 @@
       <c r="AA105"/>
       <c r="AB105"/>
     </row>
-    <row r="106" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F106" s="21"/>
       <c r="G106" s="21"/>
       <c r="J106"/>
@@ -3952,7 +4758,7 @@
       <c r="AA106"/>
       <c r="AB106"/>
     </row>
-    <row r="107" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F107" s="21"/>
       <c r="G107" s="21"/>
       <c r="J107"/>
@@ -3975,7 +4781,7 @@
       <c r="AA107"/>
       <c r="AB107"/>
     </row>
-    <row r="108" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F108" s="21"/>
       <c r="G108" s="21"/>
       <c r="J108"/>
@@ -3998,7 +4804,7 @@
       <c r="AA108"/>
       <c r="AB108"/>
     </row>
-    <row r="109" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F109" s="21"/>
       <c r="G109" s="21"/>
       <c r="J109"/>
@@ -4021,7 +4827,7 @@
       <c r="AA109"/>
       <c r="AB109"/>
     </row>
-    <row r="110" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F110" s="21"/>
       <c r="G110" s="21"/>
       <c r="J110"/>
@@ -4044,7 +4850,7 @@
       <c r="AA110"/>
       <c r="AB110"/>
     </row>
-    <row r="111" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F111" s="21"/>
       <c r="G111" s="21"/>
       <c r="J111"/>
@@ -4067,7 +4873,7 @@
       <c r="AA111"/>
       <c r="AB111"/>
     </row>
-    <row r="112" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F112" s="21"/>
       <c r="G112" s="21"/>
       <c r="J112"/>
@@ -4090,7 +4896,7 @@
       <c r="AA112"/>
       <c r="AB112"/>
     </row>
-    <row r="113" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F113" s="21"/>
       <c r="G113" s="21"/>
       <c r="J113"/>
@@ -4113,7 +4919,7 @@
       <c r="AA113"/>
       <c r="AB113"/>
     </row>
-    <row r="114" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J114"/>
       <c r="K114"/>
       <c r="L114"/>
@@ -4134,7 +4940,7 @@
       <c r="AA114"/>
       <c r="AB114"/>
     </row>
-    <row r="115" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I115"/>
       <c r="J115"/>
       <c r="K115"/>
@@ -4156,7 +4962,7 @@
       <c r="AA115"/>
       <c r="AB115"/>
     </row>
-    <row r="116" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I116"/>
       <c r="J116"/>
       <c r="K116"/>
@@ -4178,7 +4984,7 @@
       <c r="AA116"/>
       <c r="AB116"/>
     </row>
-    <row r="117" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I117"/>
       <c r="J117"/>
       <c r="K117"/>
@@ -4200,7 +5006,7 @@
       <c r="AA117"/>
       <c r="AB117"/>
     </row>
-    <row r="118" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I118"/>
       <c r="J118"/>
       <c r="K118"/>
@@ -4222,7 +5028,7 @@
       <c r="AA118"/>
       <c r="AB118"/>
     </row>
-    <row r="119" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I119"/>
       <c r="J119"/>
       <c r="K119"/>
@@ -4244,7 +5050,7 @@
       <c r="AA119"/>
       <c r="AB119"/>
     </row>
-    <row r="120" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I120"/>
       <c r="J120"/>
       <c r="K120"/>
@@ -4266,7 +5072,7 @@
       <c r="AA120"/>
       <c r="AB120"/>
     </row>
-    <row r="121" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I121"/>
       <c r="J121"/>
       <c r="K121"/>
@@ -4288,7 +5094,7 @@
       <c r="AA121"/>
       <c r="AB121"/>
     </row>
-    <row r="122" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I122"/>
       <c r="J122"/>
       <c r="K122"/>
@@ -4310,7 +5116,7 @@
       <c r="AA122"/>
       <c r="AB122"/>
     </row>
-    <row r="123" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I123"/>
       <c r="J123"/>
       <c r="K123"/>
@@ -4332,7 +5138,7 @@
       <c r="AA123"/>
       <c r="AB123"/>
     </row>
-    <row r="124" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I124"/>
       <c r="J124"/>
       <c r="K124"/>
@@ -4354,7 +5160,7 @@
       <c r="AA124"/>
       <c r="AB124"/>
     </row>
-    <row r="125" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I125"/>
       <c r="J125"/>
       <c r="K125"/>
@@ -4376,7 +5182,7 @@
       <c r="AA125"/>
       <c r="AB125"/>
     </row>
-    <row r="126" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I126"/>
       <c r="J126"/>
       <c r="K126"/>
@@ -4398,7 +5204,7 @@
       <c r="AA126"/>
       <c r="AB126"/>
     </row>
-    <row r="127" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I127"/>
       <c r="J127"/>
       <c r="K127"/>
@@ -4420,7 +5226,7 @@
       <c r="AA127"/>
       <c r="AB127"/>
     </row>
-    <row r="128" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="6:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I128"/>
       <c r="J128"/>
       <c r="K128"/>
@@ -4442,7 +5248,7 @@
       <c r="AA128"/>
       <c r="AB128"/>
     </row>
-    <row r="129" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I129"/>
       <c r="J129"/>
       <c r="K129"/>
@@ -4464,7 +5270,7 @@
       <c r="AA129"/>
       <c r="AB129"/>
     </row>
-    <row r="130" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="130" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I130"/>
       <c r="J130"/>
       <c r="K130"/>
@@ -4486,7 +5292,7 @@
       <c r="AA130"/>
       <c r="AB130"/>
     </row>
-    <row r="131" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="131" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I131"/>
       <c r="J131"/>
       <c r="K131"/>
@@ -4508,7 +5314,7 @@
       <c r="AA131"/>
       <c r="AB131"/>
     </row>
-    <row r="132" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="132" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I132"/>
       <c r="J132"/>
       <c r="K132"/>
@@ -4530,7 +5336,7 @@
       <c r="AA132"/>
       <c r="AB132"/>
     </row>
-    <row r="133" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I133"/>
       <c r="J133"/>
       <c r="K133"/>
@@ -4552,7 +5358,7 @@
       <c r="AA133"/>
       <c r="AB133"/>
     </row>
-    <row r="134" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="134" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I134"/>
       <c r="J134"/>
       <c r="K134"/>
@@ -4574,7 +5380,7 @@
       <c r="AA134"/>
       <c r="AB134"/>
     </row>
-    <row r="135" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I135"/>
       <c r="J135"/>
       <c r="K135"/>
@@ -4596,7 +5402,7 @@
       <c r="AA135"/>
       <c r="AB135"/>
     </row>
-    <row r="136" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I136"/>
       <c r="J136"/>
       <c r="K136"/>
@@ -4618,7 +5424,7 @@
       <c r="AA136"/>
       <c r="AB136"/>
     </row>
-    <row r="137" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I137"/>
       <c r="J137"/>
       <c r="K137"/>
@@ -4640,7 +5446,7 @@
       <c r="AA137"/>
       <c r="AB137"/>
     </row>
-    <row r="138" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I138"/>
       <c r="J138"/>
       <c r="K138"/>
@@ -4662,7 +5468,7 @@
       <c r="AA138"/>
       <c r="AB138"/>
     </row>
-    <row r="139" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I139"/>
       <c r="J139"/>
       <c r="K139"/>
@@ -4684,7 +5490,7 @@
       <c r="AA139"/>
       <c r="AB139"/>
     </row>
-    <row r="140" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I140"/>
       <c r="J140"/>
       <c r="K140"/>
@@ -4706,7 +5512,7 @@
       <c r="AA140"/>
       <c r="AB140"/>
     </row>
-    <row r="141" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I141"/>
       <c r="J141"/>
       <c r="K141"/>
@@ -4728,7 +5534,7 @@
       <c r="AA141"/>
       <c r="AB141"/>
     </row>
-    <row r="142" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I142"/>
       <c r="J142"/>
       <c r="K142"/>
@@ -4750,7 +5556,7 @@
       <c r="AA142"/>
       <c r="AB142"/>
     </row>
-    <row r="143" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I143"/>
       <c r="J143"/>
       <c r="K143"/>
@@ -4772,7 +5578,7 @@
       <c r="AA143"/>
       <c r="AB143"/>
     </row>
-    <row r="144" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I144"/>
       <c r="J144"/>
       <c r="K144"/>
@@ -4794,7 +5600,7 @@
       <c r="AA144"/>
       <c r="AB144"/>
     </row>
-    <row r="145" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I145"/>
       <c r="J145"/>
       <c r="K145"/>
@@ -4816,7 +5622,7 @@
       <c r="AA145"/>
       <c r="AB145"/>
     </row>
-    <row r="146" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I146"/>
       <c r="J146"/>
       <c r="K146"/>
@@ -4838,7 +5644,7 @@
       <c r="AA146"/>
       <c r="AB146"/>
     </row>
-    <row r="147" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I147"/>
       <c r="J147"/>
       <c r="K147"/>
@@ -4860,7 +5666,7 @@
       <c r="AA147"/>
       <c r="AB147"/>
     </row>
-    <row r="148" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I148"/>
       <c r="J148"/>
       <c r="K148"/>
@@ -4882,7 +5688,7 @@
       <c r="AA148"/>
       <c r="AB148"/>
     </row>
-    <row r="149" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I149"/>
       <c r="J149"/>
       <c r="K149"/>
@@ -4904,7 +5710,7 @@
       <c r="AA149"/>
       <c r="AB149"/>
     </row>
-    <row r="150" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I150"/>
       <c r="J150"/>
       <c r="K150"/>
@@ -4926,7 +5732,7 @@
       <c r="AA150"/>
       <c r="AB150"/>
     </row>
-    <row r="151" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I151"/>
       <c r="J151"/>
       <c r="K151"/>
@@ -4948,7 +5754,7 @@
       <c r="AA151"/>
       <c r="AB151"/>
     </row>
-    <row r="152" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I152"/>
       <c r="J152"/>
       <c r="K152"/>
@@ -4970,7 +5776,7 @@
       <c r="AA152"/>
       <c r="AB152"/>
     </row>
-    <row r="153" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I153"/>
       <c r="J153"/>
       <c r="K153"/>
@@ -4992,7 +5798,7 @@
       <c r="AA153"/>
       <c r="AB153"/>
     </row>
-    <row r="154" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="154" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I154"/>
       <c r="J154"/>
       <c r="K154"/>
@@ -5014,7 +5820,7 @@
       <c r="AA154"/>
       <c r="AB154"/>
     </row>
-    <row r="155" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="155" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I155"/>
       <c r="J155"/>
       <c r="K155"/>
@@ -5036,7 +5842,7 @@
       <c r="AA155"/>
       <c r="AB155"/>
     </row>
-    <row r="156" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I156"/>
       <c r="J156"/>
       <c r="K156"/>
@@ -5058,7 +5864,7 @@
       <c r="AA156"/>
       <c r="AB156"/>
     </row>
-    <row r="157" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="157" spans="9:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I157"/>
       <c r="J157"/>
       <c r="K157"/>
@@ -5082,11 +5888,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5094,37 +5895,182 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
-    <cfRule type="expression" dxfId="8" priority="29">
+    <cfRule type="expression" dxfId="48" priority="69">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BP4">
-    <cfRule type="expression" dxfId="7" priority="34">
+    <cfRule type="expression" dxfId="47" priority="74">
       <formula>I$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BP80">
-    <cfRule type="expression" dxfId="6" priority="26">
+    <cfRule type="expression" dxfId="46" priority="66">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="27">
+    <cfRule type="expression" dxfId="45" priority="67">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="28">
+    <cfRule type="expression" dxfId="44" priority="68">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="30">
+    <cfRule type="expression" dxfId="43" priority="70">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="31">
+    <cfRule type="expression" dxfId="42" priority="71">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="32">
+    <cfRule type="expression" dxfId="41" priority="72">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="33">
+    <cfRule type="expression" dxfId="40" priority="73">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81:BD81">
+    <cfRule type="expression" dxfId="39" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81:BO81">
+    <cfRule type="expression" dxfId="38" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>I$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I82:BD82">
+    <cfRule type="expression" dxfId="31" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I82:BO82">
+    <cfRule type="expression" dxfId="30" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>I$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I83:BD83">
+    <cfRule type="expression" dxfId="23" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I83:BO83">
+    <cfRule type="expression" dxfId="22" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>I$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84:BD90">
+    <cfRule type="expression" dxfId="15" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I84:BO90">
+    <cfRule type="expression" dxfId="14" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>I$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I91:BD91">
+    <cfRule type="expression" dxfId="7" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I91:BO91">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>I$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
sprint 6 management updates
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\fct-unl\INFORMATICA\5th_sem\courses\ES\project\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021BE87A-9DA9-41A1-B358-8A1EBFF21BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBBDBAA-7506-4C02-8732-D36110815D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,19 @@
     <definedName name="TitleRegion..BO60">'Project Planner'!$C$3:$C$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -829,12 +840,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -843,6 +848,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -867,7 +878,7 @@
     <cellStyle name="Plan legend" xfId="11" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="12" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -935,21 +946,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9"/>
         </patternFill>
       </fill>
@@ -989,6 +985,25 @@
         <top/>
         <bottom style="thin">
           <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="7"/>
         </bottom>
       </border>
     </dxf>
@@ -1113,506 +1128,6 @@
         <top/>
         <bottom style="thin">
           <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="9" tint="0.59978026673177287"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59978026673177287"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color theme="7"/>
         </bottom>
       </border>
     </dxf>
@@ -1897,8 +1412,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B88" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1936,69 +1451,69 @@
         <v>41</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="28"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -2073,13 +1588,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -4000,7 +3515,9 @@
       <c r="E80" s="2">
         <v>3</v>
       </c>
-      <c r="F80" s="21"/>
+      <c r="F80" s="21">
+        <v>40</v>
+      </c>
       <c r="G80" s="21"/>
       <c r="J80"/>
       <c r="K80"/>
@@ -4351,12 +3868,14 @@
         <v>114</v>
       </c>
       <c r="D90" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E90" s="2">
-        <v>2</v>
-      </c>
-      <c r="F90" s="21"/>
+        <v>3</v>
+      </c>
+      <c r="F90" s="21">
+        <v>40</v>
+      </c>
       <c r="G90" s="21"/>
       <c r="J90"/>
       <c r="K90"/>
@@ -4386,12 +3905,14 @@
         <v>115</v>
       </c>
       <c r="D91" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E91" s="2">
-        <v>2</v>
-      </c>
-      <c r="F91" s="21"/>
+        <v>3</v>
+      </c>
+      <c r="F91" s="21">
+        <v>40</v>
+      </c>
       <c r="G91" s="21"/>
       <c r="J91"/>
       <c r="K91"/>
@@ -5888,6 +5409,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5895,182 +5421,65 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
-    <cfRule type="expression" dxfId="48" priority="69">
+    <cfRule type="expression" dxfId="16" priority="69">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I81:BD91">
+    <cfRule type="expression" dxfId="15" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I81:BO91">
+    <cfRule type="expression" dxfId="14" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>I$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I4:BP4">
-    <cfRule type="expression" dxfId="47" priority="74">
+    <cfRule type="expression" dxfId="7" priority="74">
       <formula>I$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BP80">
-    <cfRule type="expression" dxfId="46" priority="66">
+    <cfRule type="expression" dxfId="6" priority="68">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="66">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="67">
+    <cfRule type="expression" dxfId="4" priority="67">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="68">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="70">
+    <cfRule type="expression" dxfId="3" priority="70">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="71">
+    <cfRule type="expression" dxfId="2" priority="71">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="72">
+    <cfRule type="expression" dxfId="1" priority="72">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="73">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81:BD81">
-    <cfRule type="expression" dxfId="39" priority="36">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I81:BO81">
-    <cfRule type="expression" dxfId="38" priority="33">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="34">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="35">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="37">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38">
-      <formula>I$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="40">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I82:BD82">
-    <cfRule type="expression" dxfId="31" priority="28">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I82:BO82">
-    <cfRule type="expression" dxfId="30" priority="25">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="26">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="27">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
-      <formula>I$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I83:BD83">
-    <cfRule type="expression" dxfId="23" priority="20">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I83:BO83">
-    <cfRule type="expression" dxfId="22" priority="17">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="18">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="19">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="22">
-      <formula>I$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="23">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84:BD90">
-    <cfRule type="expression" dxfId="15" priority="12">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I84:BO90">
-    <cfRule type="expression" dxfId="14" priority="9">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="10">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="11">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
-      <formula>I$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I91:BD91">
-    <cfRule type="expression" dxfId="7" priority="4">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I91:BO91">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>I$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="0" priority="73">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
(67286, Gabriela Silva) Updated sprint 6's third day management data
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\fct-unl\INFORMATICA\5th_sem\courses\ES\project\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBBDBAA-7506-4C02-8732-D36110815D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F644803-D6D1-4C17-80AA-A3407C6E7471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,6 +840,12 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -848,12 +854,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -946,7 +946,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -961,7 +961,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7"/>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -1412,8 +1412,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1448,72 +1448,72 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="27" t="s">
+      <c r="R2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="28" t="s">
+      <c r="AJ2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="28"/>
-      <c r="AQ2" s="28"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AQ2" s="25"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1588,13 +1588,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3664,7 +3664,12 @@
       <c r="F84" s="21">
         <v>40</v>
       </c>
-      <c r="G84" s="21"/>
+      <c r="G84" s="21">
+        <v>1</v>
+      </c>
+      <c r="H84" s="3">
+        <v>1</v>
+      </c>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84"/>
@@ -3698,8 +3703,15 @@
       <c r="E85" s="2">
         <v>3</v>
       </c>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
+      <c r="F85" s="21">
+        <v>42</v>
+      </c>
+      <c r="G85" s="21">
+        <v>1</v>
+      </c>
+      <c r="H85" s="3">
+        <v>1</v>
+      </c>
       <c r="J85"/>
       <c r="K85"/>
       <c r="L85"/>
@@ -3876,7 +3888,12 @@
       <c r="F90" s="21">
         <v>40</v>
       </c>
-      <c r="G90" s="21"/>
+      <c r="G90" s="21">
+        <v>2</v>
+      </c>
+      <c r="H90" s="3">
+        <v>1</v>
+      </c>
       <c r="J90"/>
       <c r="K90"/>
       <c r="L90"/>
@@ -3913,7 +3930,12 @@
       <c r="F91" s="21">
         <v>40</v>
       </c>
-      <c r="G91" s="21"/>
+      <c r="G91" s="21">
+        <v>2</v>
+      </c>
+      <c r="H91" s="3">
+        <v>1</v>
+      </c>
       <c r="J91"/>
       <c r="K91"/>
       <c r="L91"/>
@@ -5409,11 +5431,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5421,6 +5438,11 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="16" priority="69">
@@ -5461,14 +5483,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BP80">
-    <cfRule type="expression" dxfId="6" priority="68">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="66">
+    <cfRule type="expression" dxfId="6" priority="66">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="67">
+    <cfRule type="expression" dxfId="5" priority="67">
       <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="68">
+      <formula>Actual</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="70">
       <formula>Plan</formula>

</xml_diff>

<commit_message>
(67286, Gabriela Silva) Updating sprint 6's management data
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\fct-unl\INFORMATICA\5th_sem\courses\ES\project\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F644803-D6D1-4C17-80AA-A3407C6E7471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F46FB0D-BE2F-42AA-83F7-05327FE8B63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,12 +840,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -854,6 +848,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1412,8 +1412,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H82" sqref="H82"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A75" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1451,69 +1451,69 @@
         <v>43</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="28"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1588,13 +1588,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3592,7 +3592,12 @@
       <c r="F82" s="21">
         <v>40</v>
       </c>
-      <c r="G82" s="21"/>
+      <c r="G82" s="21">
+        <v>3</v>
+      </c>
+      <c r="H82" s="3">
+        <v>1</v>
+      </c>
       <c r="J82"/>
       <c r="K82"/>
       <c r="L82"/>
@@ -5431,6 +5436,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5438,11 +5448,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="16" priority="69">

</xml_diff>

<commit_message>
(67286, Gabriela Silva) Updating sprint 6's management data: 4th day and a bit of the 5th too
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\fct-unl\INFORMATICA\5th_sem\courses\ES\project\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F46FB0D-BE2F-42AA-83F7-05327FE8B63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F866BA5C-8F9C-4C3B-8C77-10B39B6A9694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -840,6 +840,12 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -848,12 +854,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1412,8 +1412,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A75" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1448,72 +1448,72 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="27" t="s">
+      <c r="R2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
-      <c r="AE2" s="27"/>
-      <c r="AF2" s="27"/>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="27"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="28" t="s">
+      <c r="AJ2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="28"/>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="28"/>
-      <c r="AQ2" s="28"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AQ2" s="25"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1588,13 +1588,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3555,7 +3555,12 @@
       <c r="F81" s="21">
         <v>40</v>
       </c>
-      <c r="G81" s="21"/>
+      <c r="G81" s="21">
+        <v>5</v>
+      </c>
+      <c r="H81" s="3">
+        <v>1</v>
+      </c>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81"/>
@@ -3631,7 +3636,9 @@
       <c r="E83" s="2">
         <v>1</v>
       </c>
-      <c r="F83" s="21"/>
+      <c r="F83" s="21">
+        <v>44</v>
+      </c>
       <c r="G83" s="21"/>
       <c r="J83"/>
       <c r="K83"/>
@@ -3750,7 +3757,9 @@
       <c r="E86" s="2">
         <v>3</v>
       </c>
-      <c r="F86" s="21"/>
+      <c r="F86" s="21">
+        <v>45</v>
+      </c>
       <c r="G86" s="21"/>
       <c r="J86"/>
       <c r="K86"/>
@@ -3820,7 +3829,9 @@
       <c r="E88" s="2">
         <v>4</v>
       </c>
-      <c r="F88" s="21"/>
+      <c r="F88" s="21">
+        <v>45</v>
+      </c>
       <c r="G88" s="21"/>
       <c r="J88"/>
       <c r="K88"/>
@@ -5436,11 +5447,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5448,6 +5454,11 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="16" priority="69">

</xml_diff>

<commit_message>
(67286, Gabriela Silva) Updated 5th, 6th and a bit of 7th days of sprint 6's
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\fct-unl\INFORMATICA\5th_sem\courses\ES\project\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F866BA5C-8F9C-4C3B-8C77-10B39B6A9694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE7B4D1-4233-422B-A33D-F48A02B5E7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,12 +840,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="17" applyBorder="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -854,6 +848,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="16" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1412,8 +1412,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE84" sqref="AE84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1448,72 +1448,72 @@
         <v>2</v>
       </c>
       <c r="I2" s="8">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K2" s="9"/>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
       <c r="AA2" s="12"/>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
-      <c r="AH2" s="24"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
       <c r="AI2" s="13"/>
-      <c r="AJ2" s="25" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="28"/>
     </row>
     <row r="3" spans="2:68" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -1588,13 +1588,13 @@
       </c>
     </row>
     <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="18">
         <v>1</v>
       </c>
@@ -3518,7 +3518,12 @@
       <c r="F80" s="21">
         <v>40</v>
       </c>
-      <c r="G80" s="21"/>
+      <c r="G80" s="21">
+        <v>7</v>
+      </c>
+      <c r="H80" s="3">
+        <v>1</v>
+      </c>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80"/>
@@ -3639,7 +3644,12 @@
       <c r="F83" s="21">
         <v>44</v>
       </c>
-      <c r="G83" s="21"/>
+      <c r="G83" s="21">
+        <v>3</v>
+      </c>
+      <c r="H83" s="3">
+        <v>1</v>
+      </c>
       <c r="J83"/>
       <c r="K83"/>
       <c r="L83"/>
@@ -3760,7 +3770,12 @@
       <c r="F86" s="21">
         <v>45</v>
       </c>
-      <c r="G86" s="21"/>
+      <c r="G86" s="21">
+        <v>2</v>
+      </c>
+      <c r="H86" s="3">
+        <v>1</v>
+      </c>
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86"/>
@@ -3794,7 +3809,9 @@
       <c r="E87" s="2">
         <v>3</v>
       </c>
-      <c r="F87" s="21"/>
+      <c r="F87" s="21">
+        <v>47</v>
+      </c>
       <c r="G87" s="21"/>
       <c r="J87"/>
       <c r="K87"/>
@@ -3866,8 +3883,15 @@
       <c r="E89" s="2">
         <v>4</v>
       </c>
-      <c r="F89" s="21"/>
-      <c r="G89" s="21"/>
+      <c r="F89" s="21">
+        <v>46</v>
+      </c>
+      <c r="G89" s="21">
+        <v>1</v>
+      </c>
+      <c r="H89" s="3">
+        <v>1</v>
+      </c>
       <c r="J89"/>
       <c r="K89"/>
       <c r="L89"/>
@@ -5447,6 +5471,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B3:B4"/>
@@ -5454,11 +5483,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AJ2:AQ2"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
     <cfRule type="expression" dxfId="16" priority="69">

</xml_diff>

<commit_message>
(67286, Gabriela Silva) Added 7th day updates from sprint 6. Updated sprint6's readme file. Sprint done.
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\fct-unl\INFORMATICA\5th_sem\courses\ES\project\SE2526_67775_67804_67286_68130_68547_67763\SE202526\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE7B4D1-4233-422B-A33D-F48A02B5E7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96D7D39-A67D-4C0B-9CF0-1BB50EE69C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -878,7 +878,379 @@
     <cellStyle name="Plan legend" xfId="11" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Project Headers" xfId="12" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="9" tint="0.59978026673177287"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="9" tint="0.59978026673177287"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59978026673177287"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color theme="9" tint="0.59978026673177287"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1412,8 +1784,8 @@
   </sheetPr>
   <dimension ref="B1:BP157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE84" sqref="AE84"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A71" zoomScale="62" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR92" sqref="AR92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3812,7 +4184,12 @@
       <c r="F87" s="21">
         <v>47</v>
       </c>
-      <c r="G87" s="21"/>
+      <c r="G87" s="21">
+        <v>1</v>
+      </c>
+      <c r="H87" s="3">
+        <v>1</v>
+      </c>
       <c r="J87"/>
       <c r="K87"/>
       <c r="L87"/>
@@ -3849,7 +4226,12 @@
       <c r="F88" s="21">
         <v>45</v>
       </c>
-      <c r="G88" s="21"/>
+      <c r="G88" s="21">
+        <v>2</v>
+      </c>
+      <c r="H88" s="3">
+        <v>1</v>
+      </c>
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88"/>
@@ -5485,40 +5867,40 @@
     <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:BD80">
-    <cfRule type="expression" dxfId="16" priority="69">
+    <cfRule type="expression" dxfId="23" priority="69">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81:BD91">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="39" priority="4">
       <formula>ActualBeyond</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I81:BO91">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="37" priority="2">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="36" priority="3">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="35" priority="5">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="34" priority="6">
       <formula>I$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="33" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="32" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BP4">
-    <cfRule type="expression" dxfId="7" priority="74">
+    <cfRule type="expression" dxfId="31" priority="74">
       <formula>I$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
adds management update for sprint 7
</commit_message>
<xml_diff>
--- a/SE202526/Management/Gantt chart.xlsx
+++ b/SE202526/Management/Gantt chart.xlsx
@@ -518,7 +518,7 @@
     <numFmt numFmtId="167" formatCode="0"/>
     <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.2497"/>
@@ -624,13 +624,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <color theme="7"/>
-      <name val="Corbel"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -853,11 +846,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -881,11 +878,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="4" borderId="3" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="4" borderId="3" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="30" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="30" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -893,19 +890,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -913,7 +910,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -929,7 +926,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -937,7 +934,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -949,7 +946,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -957,19 +954,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="26" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1532,2597 +1525,2751 @@
   </sheetPr>
   <dimension ref="B1:BP113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="62" zoomScaleNormal="62" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D92" activeCellId="0" sqref="D92"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="22" zoomScaleNormal="22" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="GE72" activeCellId="0" sqref="GE72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.2578125" defaultRowHeight="30" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="2" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="15.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="9" style="2" width="3.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="78.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="3" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="15.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="9" style="3" width="3.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="8" t="n">
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="9" t="n">
         <v>47</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="10" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="10" t="s">
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="10" t="s">
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="15" t="s">
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-    </row>
-    <row r="3" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="17" t="s">
+      <c r="AK2" s="16"/>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="16"/>
+      <c r="AN2" s="16"/>
+      <c r="AO2" s="16"/>
+      <c r="AP2" s="16"/>
+      <c r="AQ2" s="16"/>
+    </row>
+    <row r="3" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="22"/>
-      <c r="Z3" s="23" t="s">
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Z3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AB3" s="22" t="s">
+      <c r="AB3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="AI3" s="22" t="s">
+      <c r="AI3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="22"/>
-      <c r="AL3" s="22"/>
-      <c r="AM3" s="22"/>
-      <c r="AN3" s="23" t="s">
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="23"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AO3" s="22"/>
-      <c r="AP3" s="22" t="s">
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AQ3" s="22"/>
-      <c r="AR3" s="22"/>
-      <c r="AS3" s="22"/>
-      <c r="AT3" s="22"/>
-      <c r="AU3" s="22"/>
-      <c r="AV3" s="22"/>
-      <c r="AW3" s="22" t="s">
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="23"/>
+      <c r="AW3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="AX3" s="22"/>
-      <c r="AY3" s="22"/>
-      <c r="AZ3" s="22"/>
-      <c r="BA3" s="22"/>
-      <c r="BB3" s="22"/>
-      <c r="BC3" s="22"/>
-      <c r="BD3" s="22" t="s">
+      <c r="AX3" s="23"/>
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="23"/>
+      <c r="BB3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BD3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="BE3" s="22"/>
-      <c r="BF3" s="22"/>
-      <c r="BG3" s="22"/>
-      <c r="BH3" s="22"/>
-      <c r="BI3" s="22"/>
-      <c r="BJ3" s="22"/>
-      <c r="BK3" s="22"/>
-      <c r="BL3" s="22"/>
-      <c r="BM3" s="22"/>
-      <c r="BN3" s="23" t="s">
+      <c r="BE3" s="23"/>
+      <c r="BF3" s="23"/>
+      <c r="BG3" s="23"/>
+      <c r="BH3" s="23"/>
+      <c r="BI3" s="23"/>
+      <c r="BJ3" s="23"/>
+      <c r="BK3" s="23"/>
+      <c r="BL3" s="23"/>
+      <c r="BM3" s="23"/>
+      <c r="BN3" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="L4" s="24" t="n">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="L4" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="M4" s="24" t="n">
+      <c r="M4" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="N4" s="24" t="n">
+      <c r="N4" s="25" t="n">
         <v>6</v>
       </c>
-      <c r="O4" s="24" t="n">
+      <c r="O4" s="25" t="n">
         <v>7</v>
       </c>
-      <c r="P4" s="24" t="n">
+      <c r="P4" s="25" t="n">
         <v>8</v>
       </c>
-      <c r="Q4" s="24" t="n">
+      <c r="Q4" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="R4" s="24" t="n">
+      <c r="R4" s="25" t="n">
         <v>10</v>
       </c>
-      <c r="S4" s="24" t="n">
+      <c r="S4" s="25" t="n">
         <v>11</v>
       </c>
-      <c r="T4" s="24" t="n">
+      <c r="T4" s="25" t="n">
         <v>12</v>
       </c>
-      <c r="U4" s="24" t="n">
+      <c r="U4" s="25" t="n">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="n">
+      <c r="V4" s="25" t="n">
         <v>14</v>
       </c>
-      <c r="W4" s="24" t="n">
+      <c r="W4" s="25" t="n">
         <v>15</v>
       </c>
-      <c r="X4" s="24" t="n">
+      <c r="X4" s="25" t="n">
         <v>16</v>
       </c>
-      <c r="Y4" s="24" t="n">
+      <c r="Y4" s="25" t="n">
         <v>17</v>
       </c>
-      <c r="Z4" s="24" t="n">
+      <c r="Z4" s="25" t="n">
         <v>18</v>
       </c>
-      <c r="AA4" s="24" t="n">
+      <c r="AA4" s="25" t="n">
         <v>19</v>
       </c>
-      <c r="AB4" s="24" t="n">
+      <c r="AB4" s="25" t="n">
         <v>20</v>
       </c>
-      <c r="AC4" s="24" t="n">
+      <c r="AC4" s="25" t="n">
         <v>21</v>
       </c>
-      <c r="AD4" s="24" t="n">
+      <c r="AD4" s="25" t="n">
         <v>22</v>
       </c>
-      <c r="AE4" s="24" t="n">
+      <c r="AE4" s="25" t="n">
         <v>23</v>
       </c>
-      <c r="AF4" s="24" t="n">
+      <c r="AF4" s="25" t="n">
         <v>24</v>
       </c>
-      <c r="AG4" s="24" t="n">
+      <c r="AG4" s="25" t="n">
         <v>25</v>
       </c>
-      <c r="AH4" s="24" t="n">
+      <c r="AH4" s="25" t="n">
         <v>26</v>
       </c>
-      <c r="AI4" s="24" t="n">
+      <c r="AI4" s="25" t="n">
         <v>27</v>
       </c>
-      <c r="AJ4" s="24" t="n">
+      <c r="AJ4" s="25" t="n">
         <v>28</v>
       </c>
-      <c r="AK4" s="24" t="n">
+      <c r="AK4" s="25" t="n">
         <v>29</v>
       </c>
-      <c r="AL4" s="24" t="n">
+      <c r="AL4" s="25" t="n">
         <v>30</v>
       </c>
-      <c r="AM4" s="24" t="n">
+      <c r="AM4" s="25" t="n">
         <v>31</v>
       </c>
-      <c r="AN4" s="24" t="n">
+      <c r="AN4" s="25" t="n">
         <v>32</v>
       </c>
-      <c r="AO4" s="24" t="n">
+      <c r="AO4" s="25" t="n">
         <v>33</v>
       </c>
-      <c r="AP4" s="24" t="n">
+      <c r="AP4" s="25" t="n">
         <v>34</v>
       </c>
-      <c r="AQ4" s="24" t="n">
+      <c r="AQ4" s="25" t="n">
         <v>35</v>
       </c>
-      <c r="AR4" s="24" t="n">
+      <c r="AR4" s="25" t="n">
         <v>36</v>
       </c>
-      <c r="AS4" s="24" t="n">
+      <c r="AS4" s="25" t="n">
         <v>37</v>
       </c>
-      <c r="AT4" s="24" t="n">
+      <c r="AT4" s="25" t="n">
         <v>38</v>
       </c>
-      <c r="AU4" s="24" t="n">
+      <c r="AU4" s="25" t="n">
         <v>39</v>
       </c>
-      <c r="AV4" s="24" t="n">
+      <c r="AV4" s="25" t="n">
         <v>40</v>
       </c>
-      <c r="AW4" s="24" t="n">
+      <c r="AW4" s="25" t="n">
         <v>41</v>
       </c>
-      <c r="AX4" s="24" t="n">
+      <c r="AX4" s="25" t="n">
         <v>42</v>
       </c>
-      <c r="AY4" s="24" t="n">
+      <c r="AY4" s="25" t="n">
         <v>43</v>
       </c>
-      <c r="AZ4" s="24" t="n">
+      <c r="AZ4" s="25" t="n">
         <v>44</v>
       </c>
-      <c r="BA4" s="24" t="n">
+      <c r="BA4" s="25" t="n">
         <v>45</v>
       </c>
-      <c r="BB4" s="24" t="n">
+      <c r="BB4" s="25" t="n">
         <v>46</v>
       </c>
-      <c r="BC4" s="24" t="n">
+      <c r="BC4" s="25" t="n">
         <v>47</v>
       </c>
-      <c r="BD4" s="24" t="n">
+      <c r="BD4" s="25" t="n">
         <v>48</v>
       </c>
-      <c r="BE4" s="24" t="n">
+      <c r="BE4" s="25" t="n">
         <v>49</v>
       </c>
-      <c r="BF4" s="24" t="n">
+      <c r="BF4" s="25" t="n">
         <v>50</v>
       </c>
-      <c r="BG4" s="24" t="n">
+      <c r="BG4" s="25" t="n">
         <v>51</v>
       </c>
-      <c r="BH4" s="24" t="n">
+      <c r="BH4" s="25" t="n">
         <v>52</v>
       </c>
-      <c r="BI4" s="24" t="n">
+      <c r="BI4" s="25" t="n">
         <v>53</v>
       </c>
-      <c r="BJ4" s="24" t="n">
+      <c r="BJ4" s="25" t="n">
         <v>54</v>
       </c>
-      <c r="BK4" s="24" t="n">
+      <c r="BK4" s="25" t="n">
         <v>55</v>
       </c>
-      <c r="BL4" s="24" t="n">
+      <c r="BL4" s="25" t="n">
         <v>56</v>
       </c>
-      <c r="BM4" s="24" t="n">
+      <c r="BM4" s="25" t="n">
         <v>57</v>
       </c>
-      <c r="BN4" s="24" t="n">
+      <c r="BN4" s="25" t="n">
         <v>58</v>
       </c>
-      <c r="BO4" s="24" t="n">
+      <c r="BO4" s="25" t="n">
         <v>59</v>
       </c>
-      <c r="BP4" s="24" t="n">
+      <c r="BP4" s="25" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="27" t="n">
+      <c r="D5" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F5" s="27" t="n">
+      <c r="E5" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="27" t="n">
+      <c r="G5" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="H5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="28"/>
+      <c r="H5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="29"/>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="27" t="n">
+      <c r="D6" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="F6" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="27" t="n">
+      <c r="F6" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="28" t="n">
         <v>16</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="27" t="n">
+      <c r="D7" s="28" t="n">
         <v>8</v>
       </c>
-      <c r="E7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" s="27" t="n">
+      <c r="E7" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="27" t="n">
+      <c r="D8" s="28" t="n">
         <v>9</v>
       </c>
-      <c r="E8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="27" t="n">
+      <c r="E8" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="G8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="n">
+      <c r="G8" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="27" t="n">
+      <c r="D9" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="E9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="27" t="n">
+      <c r="E9" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="28" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="27" t="n">
+      <c r="G9" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="27" t="n">
+      <c r="D10" s="28" t="n">
         <v>11</v>
       </c>
-      <c r="E10" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" s="27" t="n">
+      <c r="E10" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="G10" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="n">
+      <c r="G10" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="27" t="n">
+      <c r="D11" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="E11" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" s="27" t="n">
+      <c r="E11" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="G11" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="n">
+      <c r="G11" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="27" t="n">
+      <c r="D12" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="E12" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" s="27" t="n">
+      <c r="E12" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="G12" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H12" s="3" t="n">
+      <c r="G12" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="27" t="n">
+      <c r="D13" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="E13" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F13" s="27" t="n">
+      <c r="E13" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="28" t="n">
         <v>17</v>
       </c>
-      <c r="G13" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="n">
+      <c r="G13" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="27" t="n">
+      <c r="D14" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="E14" s="27" t="n">
+      <c r="E14" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="F14" s="27" t="n">
+      <c r="F14" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="G14" s="27" t="n">
+      <c r="G14" s="28" t="n">
         <v>14</v>
       </c>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="4" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="27" t="n">
+      <c r="D15" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="E15" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F15" s="27" t="n">
+      <c r="E15" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="G15" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="n">
+      <c r="G15" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="27" t="n">
+      <c r="D16" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="E16" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F16" s="27" t="n">
+      <c r="E16" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="G16" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3" t="n">
+      <c r="G16" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="27" t="n">
+      <c r="D17" s="28" t="n">
         <v>14</v>
       </c>
-      <c r="E17" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F17" s="27" t="n">
+      <c r="E17" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="28" t="n">
         <v>15</v>
       </c>
-      <c r="G17" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3" t="n">
+      <c r="G17" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="27" t="n">
+      <c r="D18" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E18" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F18" s="27" t="n">
+      <c r="E18" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="G18" s="27" t="n">
+      <c r="G18" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="H18" s="3" t="n">
+      <c r="H18" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="27" t="n">
+      <c r="D19" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E19" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F19" s="27" t="n">
+      <c r="E19" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="G19" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H19" s="3" t="n">
+      <c r="G19" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="27" t="n">
+      <c r="D20" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E20" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F20" s="27" t="n">
+      <c r="E20" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="G20" s="27" t="n">
+      <c r="G20" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="H20" s="3" t="n">
+      <c r="H20" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="27" t="n">
+      <c r="D21" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E21" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F21" s="27" t="n">
+      <c r="E21" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="G21" s="27" t="n">
+      <c r="G21" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="H21" s="3" t="n">
+      <c r="H21" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="27" t="n">
+      <c r="D22" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E22" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F22" s="27" t="n">
+      <c r="E22" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="G22" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H22" s="3" t="n">
+      <c r="G22" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H22" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="27" t="n">
+      <c r="D23" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E23" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F23" s="27" t="n">
+      <c r="E23" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="G23" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H23" s="3" t="n">
+      <c r="G23" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="27" t="n">
+      <c r="D24" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="E24" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F24" s="27" t="n">
+      <c r="E24" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="G24" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24" s="3" t="n">
+      <c r="G24" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="27" t="n">
+      <c r="D25" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="E25" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F25" s="27" t="n">
+      <c r="E25" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F25" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="G25" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H25" s="3" t="n">
+      <c r="G25" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H25" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="27" t="n">
+      <c r="D26" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="E26" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F26" s="27" t="n">
+      <c r="E26" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F26" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="G26" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H26" s="3" t="n">
+      <c r="G26" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H26" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="27" t="n">
+      <c r="D27" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="E27" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F27" s="27" t="n">
+      <c r="E27" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F27" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="G27" s="27" t="n">
+      <c r="G27" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="H27" s="3" t="n">
+      <c r="H27" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="27" t="n">
+      <c r="D28" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="E28" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F28" s="27" t="n">
+      <c r="E28" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F28" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="G28" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="3" t="n">
+      <c r="G28" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="27" t="n">
+      <c r="D29" s="28" t="n">
         <v>22</v>
       </c>
-      <c r="E29" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F29" s="27" t="n">
+      <c r="E29" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F29" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="G29" s="27" t="n">
+      <c r="G29" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="H29" s="3" t="n">
+      <c r="H29" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="27" t="n">
+      <c r="D30" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E30" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F30" s="27" t="n">
+      <c r="E30" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="G30" s="27" t="n">
+      <c r="G30" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="H30" s="3" t="n">
+      <c r="H30" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="27" t="n">
+      <c r="D31" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E31" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F31" s="27" t="n">
+      <c r="E31" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="G31" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H31" s="3" t="n">
+      <c r="G31" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H31" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="27" t="n">
+      <c r="D32" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E32" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F32" s="27" t="n">
+      <c r="E32" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="G32" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H32" s="3" t="n">
+      <c r="G32" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H32" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="27" t="n">
+      <c r="D33" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E33" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F33" s="27" t="n">
+      <c r="E33" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="G33" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H33" s="3" t="n">
+      <c r="G33" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H33" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="27" t="n">
+      <c r="D34" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E34" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F34" s="27" t="n">
+      <c r="E34" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F34" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="G34" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H34" s="3" t="n">
+      <c r="G34" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="27" t="n">
+      <c r="D35" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E35" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F35" s="27" t="n">
+      <c r="E35" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F35" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="G35" s="27" t="n">
+      <c r="G35" s="28" t="n">
         <v>8</v>
       </c>
-      <c r="H35" s="3" t="n">
+      <c r="H35" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="27" t="n">
+      <c r="D36" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E36" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F36" s="27" t="n">
+      <c r="E36" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="G36" s="27" t="n">
+      <c r="G36" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="H36" s="3" t="n">
+      <c r="H36" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="27" t="n">
+      <c r="D37" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E37" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F37" s="27" t="n">
+      <c r="E37" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="G37" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H37" s="3" t="n">
+      <c r="G37" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H37" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="27" t="n">
+      <c r="D38" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E38" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F38" s="27" t="n">
+      <c r="E38" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F38" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="G38" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H38" s="3" t="n">
+      <c r="G38" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H38" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="27" t="n">
+      <c r="D39" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E39" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F39" s="27" t="n">
+      <c r="E39" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="G39" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H39" s="3" t="n">
+      <c r="G39" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H39" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="27" t="n">
+      <c r="D40" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E40" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F40" s="27" t="n">
+      <c r="E40" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="G40" s="27" t="n">
+      <c r="G40" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="H40" s="3" t="n">
+      <c r="H40" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="27" t="n">
+      <c r="D41" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="E41" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F41" s="27" t="n">
+      <c r="E41" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F41" s="28" t="n">
         <v>21</v>
       </c>
-      <c r="G41" s="27" t="n">
+      <c r="G41" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="H41" s="3" t="n">
+      <c r="H41" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="27" t="n">
+      <c r="D42" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="E42" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F42" s="27" t="n">
+      <c r="E42" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F42" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="G42" s="27" t="n">
+      <c r="G42" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="H42" s="3" t="n">
+      <c r="H42" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="27" t="n">
+      <c r="D43" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="E43" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F43" s="27" t="n">
+      <c r="E43" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F43" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="G43" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H43" s="3" t="n">
+      <c r="G43" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H43" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="27" t="n">
+      <c r="D44" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="E44" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F44" s="27" t="n">
+      <c r="E44" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F44" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="G44" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H44" s="3" t="n">
+      <c r="G44" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H44" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="27" t="n">
+      <c r="D45" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="E45" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F45" s="27" t="n">
+      <c r="E45" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F45" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="G45" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H45" s="3" t="n">
+      <c r="G45" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H45" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="27" t="n">
+      <c r="D46" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="E46" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F46" s="27" t="n">
+      <c r="E46" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F46" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="G46" s="27" t="n">
+      <c r="G46" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="H46" s="3" t="n">
+      <c r="H46" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="27" t="n">
+      <c r="D47" s="28" t="n">
         <v>23</v>
       </c>
-      <c r="E47" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F47" s="27" t="n">
+      <c r="E47" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F47" s="28" t="n">
         <v>24</v>
       </c>
-      <c r="G47" s="27" t="n">
+      <c r="G47" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="H47" s="3" t="n">
+      <c r="H47" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="27" t="n">
+      <c r="D48" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E48" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" s="27" t="n">
+      <c r="E48" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G48" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H48" s="3" t="n">
+      <c r="G48" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="n">
+      <c r="B49" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D49" s="27" t="n">
+      <c r="D49" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E49" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" s="27" t="n">
+      <c r="E49" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" s="28" t="n">
         <v>31</v>
       </c>
-      <c r="G49" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H49" s="3" t="n">
+      <c r="G49" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D50" s="27" t="n">
+      <c r="D50" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E50" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F50" s="27" t="n">
+      <c r="E50" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="28" t="n">
         <v>31</v>
       </c>
-      <c r="G50" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H50" s="3" t="n">
+      <c r="G50" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="27" t="n">
+      <c r="D51" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E51" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F51" s="27" t="n">
+      <c r="E51" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G51" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H51" s="3" t="n">
+      <c r="G51" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="n">
+      <c r="B52" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D52" s="27" t="n">
+      <c r="D52" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E52" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F52" s="27" t="n">
+      <c r="E52" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G52" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H52" s="3" t="n">
+      <c r="G52" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="n">
+      <c r="B53" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D53" s="27" t="n">
+      <c r="D53" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E53" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F53" s="27" t="n">
+      <c r="E53" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G53" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H53" s="3" t="n">
+      <c r="G53" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="n">
+      <c r="B54" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C54" s="26" t="s">
+      <c r="C54" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="D54" s="27" t="n">
+      <c r="D54" s="28" t="n">
         <v>31</v>
       </c>
-      <c r="E54" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F54" s="27" t="n">
+      <c r="E54" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F54" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G54" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H54" s="3" t="n">
+      <c r="G54" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="n">
+      <c r="B55" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D55" s="27" t="n">
+      <c r="D55" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E55" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F55" s="27" t="n">
+      <c r="E55" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G55" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H55" s="3" t="n">
+      <c r="G55" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="n">
+      <c r="B56" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C56" s="26" t="s">
+      <c r="C56" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="27" t="n">
+      <c r="D56" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E56" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F56" s="27" t="n">
+      <c r="E56" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G56" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H56" s="3" t="n">
+      <c r="G56" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="n">
+      <c r="B57" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D57" s="27" t="n">
+      <c r="D57" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E57" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F57" s="27" t="n">
+      <c r="E57" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G57" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H57" s="3" t="n">
+      <c r="G57" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="D58" s="27" t="n">
+      <c r="D58" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E58" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F58" s="27" t="n">
+      <c r="E58" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F58" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G58" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H58" s="3" t="n">
+      <c r="G58" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D59" s="27" t="n">
+      <c r="D59" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="E59" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F59" s="27" t="n">
+      <c r="E59" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G59" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H59" s="3" t="n">
+      <c r="G59" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D60" s="27" t="n">
+      <c r="D60" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="E60" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F60" s="27" t="n">
+      <c r="E60" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="G60" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H60" s="3" t="n">
+      <c r="G60" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="n">
+      <c r="B61" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D61" s="27" t="n">
+      <c r="D61" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="E61" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F61" s="27" t="n">
+      <c r="E61" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="G61" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H61" s="3" t="n">
+      <c r="G61" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H61" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="n">
+      <c r="B62" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D62" s="27" t="n">
+      <c r="D62" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="E62" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" s="27" t="n">
+      <c r="E62" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="G62" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H62" s="3" t="n">
+      <c r="G62" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H62" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="C63" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D63" s="27" t="n">
+      <c r="D63" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="E63" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F63" s="27" t="n">
+      <c r="E63" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="G63" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H63" s="3" t="n">
+      <c r="G63" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0" t="n">
+      <c r="B64" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C64" s="26" t="s">
+      <c r="C64" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D64" s="27" t="n">
+      <c r="D64" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="E64" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F64" s="27" t="n">
+      <c r="E64" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="G64" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H64" s="3" t="n">
+      <c r="G64" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="n">
+      <c r="B65" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C65" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D65" s="27" t="n">
+      <c r="D65" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="E65" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F65" s="27" t="n">
+      <c r="E65" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="G65" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H65" s="3" t="n">
+      <c r="G65" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0" t="n">
+      <c r="B66" s="1" t="n">
         <v>67286</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D66" s="27" t="n">
+      <c r="D66" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="E66" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F66" s="27" t="n">
+      <c r="E66" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F66" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="G66" s="27" t="n">
+      <c r="G66" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="H66" s="3" t="n">
+      <c r="H66" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D67" s="27" t="n">
+      <c r="D67" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="E67" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F67" s="27" t="n">
+      <c r="E67" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F67" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="G67" s="27" t="n">
+      <c r="G67" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="H67" s="3" t="n">
+      <c r="H67" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0" t="n">
+      <c r="B68" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C68" s="26" t="s">
+      <c r="C68" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D68" s="27" t="n">
+      <c r="D68" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="E68" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F68" s="27" t="n">
+      <c r="E68" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F68" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="G68" s="27" t="n">
+      <c r="G68" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="H68" s="3" t="n">
+      <c r="H68" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="0" t="n">
+      <c r="B69" s="1" t="n">
         <v>67804</v>
       </c>
-      <c r="C69" s="26" t="s">
+      <c r="C69" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D69" s="27" t="n">
+      <c r="D69" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="E69" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F69" s="27" t="n">
+      <c r="E69" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F69" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="G69" s="27" t="n">
+      <c r="G69" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="H69" s="3" t="n">
+      <c r="H69" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="1" t="n">
         <v>68130</v>
       </c>
-      <c r="C70" s="26" t="s">
+      <c r="C70" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="D70" s="27" t="n">
+      <c r="D70" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="E70" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F70" s="27" t="n">
+      <c r="E70" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F70" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="G70" s="27" t="n">
+      <c r="G70" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="H70" s="3" t="n">
+      <c r="H70" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="n">
+      <c r="B71" s="1" t="n">
         <v>68547</v>
       </c>
-      <c r="C71" s="26" t="s">
+      <c r="C71" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D71" s="27" t="n">
+      <c r="D71" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="E71" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F71" s="27" t="n">
+      <c r="E71" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F71" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="G71" s="27" t="n">
+      <c r="G71" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="H71" s="3" t="n">
+      <c r="H71" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="n">
+      <c r="B72" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C72" s="26" t="s">
+      <c r="C72" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D72" s="27" t="n">
+      <c r="D72" s="28" t="n">
         <v>34</v>
       </c>
-      <c r="E72" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F72" s="27" t="n">
+      <c r="E72" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F72" s="28" t="n">
         <v>36</v>
       </c>
-      <c r="G72" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H72" s="3" t="n">
+      <c r="G72" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="n">
+      <c r="B73" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="C73" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D73" s="2" t="n">
+      <c r="D73" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="E73" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F73" s="27" t="n">
+      <c r="E73" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F73" s="28" t="n">
         <v>36</v>
       </c>
-      <c r="G73" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H73" s="3" t="n">
+      <c r="G73" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0" t="s">
+      <c r="B74" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D74" s="2" t="n">
+      <c r="D74" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="E74" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F74" s="27" t="n">
+      <c r="E74" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F74" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="G74" s="27" t="n">
+      <c r="G74" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="H74" s="29" t="n">
+      <c r="H74" s="30" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="0" t="n">
+      <c r="B75" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D75" s="2" t="n">
+      <c r="D75" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="E75" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F75" s="27" t="n">
+      <c r="E75" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" s="28" t="n">
         <v>34</v>
       </c>
-      <c r="G75" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H75" s="3" t="n">
+      <c r="G75" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="n">
+      <c r="B76" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D76" s="2" t="n">
+      <c r="D76" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="E76" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F76" s="27" t="n">
+      <c r="E76" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F76" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="G76" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H76" s="29" t="n">
+      <c r="G76" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H76" s="30" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="n">
+      <c r="B77" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D77" s="27" t="n">
+      <c r="D77" s="28" t="n">
         <v>34</v>
       </c>
-      <c r="E77" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="F77" s="27" t="n">
+      <c r="E77" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F77" s="28" t="n">
         <v>34</v>
       </c>
-      <c r="G77" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H77" s="29" t="n">
+      <c r="G77" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H77" s="30" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D78" s="2" t="n">
+      <c r="D78" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="E78" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="F78" s="27" t="n">
+      <c r="E78" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" s="28" t="n">
         <v>39</v>
       </c>
-      <c r="G78" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H78" s="3" t="n">
+      <c r="G78" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H78" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D79" s="2" t="n">
+      <c r="D79" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="E79" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F79" s="27" t="n">
+      <c r="E79" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" s="28" t="n">
         <v>39</v>
       </c>
-      <c r="G79" s="27" t="n">
+      <c r="G79" s="28" t="n">
         <v>1.5</v>
       </c>
-      <c r="H79" s="3" t="n">
+      <c r="H79" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D80" s="2" t="n">
+      <c r="D80" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="E80" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F80" s="27" t="n">
+      <c r="E80" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F80" s="28" t="n">
         <v>40</v>
       </c>
-      <c r="G80" s="27" t="n">
+      <c r="G80" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="H80" s="3" t="n">
+      <c r="H80" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D81" s="2" t="n">
+      <c r="D81" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="E81" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F81" s="27" t="n">
+      <c r="E81" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F81" s="28" t="n">
         <v>40</v>
       </c>
-      <c r="G81" s="27" t="n">
+      <c r="G81" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="H81" s="3" t="n">
+      <c r="H81" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D82" s="2" t="n">
+      <c r="D82" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="E82" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F82" s="27" t="n">
+      <c r="E82" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" s="28" t="n">
         <v>40</v>
       </c>
-      <c r="G82" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H82" s="3" t="n">
+      <c r="G82" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H82" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D83" s="2" t="n">
+      <c r="D83" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="E83" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F83" s="27" t="n">
+      <c r="E83" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F83" s="28" t="n">
         <v>44</v>
       </c>
-      <c r="G83" s="27" t="n">
-        <v>3</v>
-      </c>
-      <c r="H83" s="3" t="n">
+      <c r="G83" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H83" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0" t="n">
+      <c r="B84" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D84" s="2" t="n">
+      <c r="D84" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="E84" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F84" s="27" t="n">
+      <c r="E84" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F84" s="28" t="n">
         <v>40</v>
       </c>
-      <c r="G84" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H84" s="3" t="n">
+      <c r="G84" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="0" t="n">
+      <c r="B85" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D85" s="2" t="n">
+      <c r="D85" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="E85" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F85" s="27" t="n">
+      <c r="E85" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F85" s="28" t="n">
         <v>42</v>
       </c>
-      <c r="G85" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H85" s="3" t="n">
+      <c r="G85" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H85" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D86" s="2" t="n">
+      <c r="D86" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="E86" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F86" s="27" t="n">
+      <c r="E86" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F86" s="28" t="n">
         <v>45</v>
       </c>
-      <c r="G86" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H86" s="3" t="n">
+      <c r="G86" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H86" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D87" s="2" t="n">
+      <c r="D87" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="E87" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F87" s="27" t="n">
+      <c r="E87" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F87" s="28" t="n">
         <v>47</v>
       </c>
-      <c r="G87" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H87" s="3" t="n">
+      <c r="G87" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="0" t="n">
+      <c r="B88" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D88" s="2" t="n">
+      <c r="D88" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="E88" s="2" t="n">
+      <c r="E88" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F88" s="27" t="n">
+      <c r="F88" s="28" t="n">
         <v>45</v>
       </c>
-      <c r="G88" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H88" s="3" t="n">
+      <c r="G88" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H88" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="0" t="n">
+      <c r="B89" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D89" s="2" t="n">
+      <c r="D89" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="E89" s="2" t="n">
+      <c r="E89" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F89" s="27" t="n">
+      <c r="F89" s="28" t="n">
         <v>46</v>
       </c>
-      <c r="G89" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H89" s="3" t="n">
+      <c r="G89" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H89" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0" t="n">
+      <c r="B90" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D90" s="2" t="n">
+      <c r="D90" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="E90" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F90" s="27" t="n">
+      <c r="E90" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F90" s="28" t="n">
         <v>40</v>
       </c>
-      <c r="G90" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H90" s="3" t="n">
+      <c r="G90" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H90" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="0" t="n">
+      <c r="B91" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D91" s="2" t="n">
+      <c r="D91" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="E91" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F91" s="27" t="n">
+      <c r="E91" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F91" s="28" t="n">
         <v>40</v>
       </c>
-      <c r="G91" s="27" t="n">
-        <v>2</v>
-      </c>
-      <c r="H91" s="3" t="n">
+      <c r="G91" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H91" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B92" s="0" t="s">
+      <c r="B92" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="30" t="n">
+      <c r="D92" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="E92" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F92" s="28" t="n">
+        <v>48</v>
+      </c>
+      <c r="G92" s="28" t="n">
+        <v>9</v>
+      </c>
+      <c r="H92" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="30" t="n">
+      <c r="D93" s="3" t="n">
+        <v>49</v>
+      </c>
+      <c r="E93" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F93" s="28" t="n">
+        <v>49</v>
+      </c>
+      <c r="G93" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H93" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F94" s="27"/>
-      <c r="G94" s="27"/>
-      <c r="H94" s="30" t="n">
+      <c r="D94" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F94" s="28" t="n">
+        <v>47</v>
+      </c>
+      <c r="G94" s="28" t="n">
+        <v>8</v>
+      </c>
+      <c r="H94" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F95" s="27"/>
-      <c r="G95" s="27"/>
-      <c r="H95" s="30" t="n">
+      <c r="D95" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E95" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F95" s="28" t="n">
+        <v>51</v>
+      </c>
+      <c r="G95" s="28" t="n">
+        <v>6</v>
+      </c>
+      <c r="H95" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B96" s="0" t="n">
+      <c r="B96" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F96" s="27"/>
-      <c r="G96" s="27"/>
-      <c r="H96" s="30" t="n">
+      <c r="D96" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="E96" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F96" s="28" t="n">
+        <v>47</v>
+      </c>
+      <c r="G96" s="28" t="n">
+        <v>6</v>
+      </c>
+      <c r="H96" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="0" t="n">
+      <c r="B97" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="30" t="n">
+      <c r="D97" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="E97" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F97" s="28" t="n">
+        <v>48</v>
+      </c>
+      <c r="G97" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H97" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="30" t="n">
+      <c r="D98" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E98" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F98" s="28" t="n">
+        <v>52</v>
+      </c>
+      <c r="G98" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H98" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="30" t="n">
+      <c r="D99" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="E99" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F99" s="28" t="n">
+        <v>54</v>
+      </c>
+      <c r="G99" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H99" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0" t="n">
+      <c r="B100" s="1" t="n">
         <v>67775</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F100" s="27"/>
-      <c r="G100" s="27"/>
-      <c r="H100" s="30" t="n">
+      <c r="D100" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="E100" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F100" s="28" t="n">
+        <v>48</v>
+      </c>
+      <c r="G100" s="28" t="n">
+        <v>7</v>
+      </c>
+      <c r="H100" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="0" t="n">
+      <c r="B101" s="1" t="n">
         <v>67763</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
-      <c r="H101" s="30" t="n">
+      <c r="D101" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="E101" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F101" s="28" t="n">
+        <v>47</v>
+      </c>
+      <c r="G101" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H101" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="0" t="s">
+      <c r="B102" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
-      <c r="H102" s="30" t="n">
+      <c r="D102" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="E102" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F102" s="28" t="n">
+        <v>53</v>
+      </c>
+      <c r="G102" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H102" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F103" s="27"/>
-      <c r="G103" s="27"/>
-      <c r="H103" s="30" t="n">
+      <c r="D103" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="E103" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F103" s="28" t="n">
+        <v>48</v>
+      </c>
+      <c r="G103" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H103" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F104" s="27"/>
-      <c r="G104" s="27"/>
-      <c r="H104" s="30" t="n">
+      <c r="D104" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="E104" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F104" s="28" t="n">
+        <v>48</v>
+      </c>
+      <c r="G104" s="28" t="n">
+        <v>5</v>
+      </c>
+      <c r="H104" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F105" s="27"/>
-      <c r="G105" s="27"/>
-      <c r="H105" s="30" t="n">
+      <c r="D105" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="E105" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F105" s="28" t="n">
+        <v>55</v>
+      </c>
+      <c r="G105" s="28" t="n">
+        <v>3</v>
+      </c>
+      <c r="H105" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="0" t="s">
+      <c r="B106" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F106" s="27"/>
-      <c r="G106" s="27"/>
-      <c r="H106" s="30" t="n">
+      <c r="D106" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="E106" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F106" s="28" t="n">
+        <v>56</v>
+      </c>
+      <c r="G106" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="H106" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F107" s="27"/>
-      <c r="G107" s="27"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
     </row>
     <row r="108" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
     </row>
     <row r="109" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
+      <c r="F109" s="28"/>
+      <c r="G109" s="28"/>
     </row>
     <row r="110" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F110" s="27"/>
-      <c r="G110" s="27"/>
+      <c r="F110" s="28"/>
+      <c r="G110" s="28"/>
     </row>
     <row r="111" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F111" s="27"/>
-      <c r="G111" s="27"/>
+      <c r="F111" s="28"/>
+      <c r="G111" s="28"/>
     </row>
     <row r="112" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F112" s="27"/>
-      <c r="G112" s="27"/>
+      <c r="F112" s="28"/>
+      <c r="G112" s="28"/>
     </row>
     <row r="113" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F113" s="27"/>
-      <c r="G113" s="27"/>
+      <c r="F113" s="28"/>
+      <c r="G113" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
     <mergeCell ref="L2:P2"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="W2:Z2"/>
@@ -4135,6 +4282,10 @@
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
+    <mergeCell ref="D107:D108"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="F107:F108"/>
+    <mergeCell ref="G107:G108"/>
   </mergeCells>
   <conditionalFormatting sqref="I81:BO90 I92:BO106">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -4262,19 +4413,19 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter plan start period in column C, starting with cell C5" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D4" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter plan start period in column C, starting with cell C5" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D4 D107:D108" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter plan duration period in column D, starting with cell D5" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E4" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter plan duration period in column D, starting with cell D5" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E4 E107:E108" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter actual start period in column E, starting with cell E5" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F3:F4" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter actual start period in column E, starting with cell E5" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F3:F4 F107:F108" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter actual duration period in column F, starting with cell F5" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G3:G4" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Enter actual duration period in column F, starting with cell F5" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G3:G4 G107:G108" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>